<commit_message>
Cambiadas mil y una gráficas, pues se salían de los márgenes. Comenzado el análisis de clusters 1 de las estaciones base (caso 5). En el excel del caso5 se tiene la comparación con los casos de estudio 1-4. Añadirla.
</commit_message>
<xml_diff>
--- a/Proyecto/Caso5.xlsx
+++ b/Proyecto/Caso5.xlsx
@@ -14,13 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
-  <si>
-    <t>Media</t>
-  </si>
-  <si>
-    <t>Desv. Tip</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="21">
   <si>
     <t>Clusters 1</t>
   </si>
@@ -38,6 +32,51 @@
   </si>
   <si>
     <t>20 sensore</t>
+  </si>
+  <si>
+    <t>Caso1</t>
+  </si>
+  <si>
+    <t>Caso 3</t>
+  </si>
+  <si>
+    <t>Caso 2</t>
+  </si>
+  <si>
+    <t>Caso 4</t>
+  </si>
+  <si>
+    <t>Comparacion</t>
+  </si>
+  <si>
+    <t>Iso</t>
+  </si>
+  <si>
+    <t>Dip</t>
+  </si>
+  <si>
+    <t>5 sensores</t>
+  </si>
+  <si>
+    <t>10 sensores</t>
+  </si>
+  <si>
+    <t>20 sensores</t>
+  </si>
+  <si>
+    <t>Mejora</t>
+  </si>
+  <si>
+    <t>Caso4</t>
+  </si>
+  <si>
+    <t>Caso3</t>
+  </si>
+  <si>
+    <t>Caso2</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
@@ -397,14 +436,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D6:AS91"/>
+  <dimension ref="D2:BI91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AJ38" sqref="AJ38:AQ38"/>
+    <sheetView tabSelected="1" topLeftCell="AO10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AU41" sqref="AU41:BB41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="35" max="35" width="13.42578125" customWidth="1"/>
     <col min="38" max="38" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -412,28 +452,109 @@
     <col min="42" max="43" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="13" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="4:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:61" x14ac:dyDescent="0.25">
+      <c r="BH2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="4:61" x14ac:dyDescent="0.25">
+      <c r="BH3" t="s">
+        <v>11</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="4:61" x14ac:dyDescent="0.25">
+      <c r="BG4" t="s">
+        <v>13</v>
+      </c>
+      <c r="BH4">
+        <v>4.5340149921451269</v>
+      </c>
+      <c r="BI4">
+        <v>4.5205202935934148</v>
+      </c>
+    </row>
+    <row r="5" spans="4:61" x14ac:dyDescent="0.25">
+      <c r="BG5" t="s">
+        <v>14</v>
+      </c>
+      <c r="BH5">
+        <v>10.126514001709587</v>
+      </c>
+      <c r="BI5">
+        <v>10.063961470180555</v>
+      </c>
+    </row>
+    <row r="6" spans="4:61" x14ac:dyDescent="0.25">
       <c r="AF6" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>1</v>
       </c>
       <c r="AJ6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG6" t="s">
+        <v>15</v>
+      </c>
+      <c r="BH6">
+        <v>19.104781491799571</v>
+      </c>
+      <c r="BI6">
+        <v>18.904530166296727</v>
+      </c>
+    </row>
+    <row r="7" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AF7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AF7" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK7" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AI7" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK7" s="2"/>
+      <c r="AL7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM7" s="2"/>
+      <c r="AN7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AO7" s="1"/>
+      <c r="AP7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AX7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AZ7" t="s">
+        <v>8</v>
+      </c>
+      <c r="BB7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>4.1397369554959296</v>
       </c>
@@ -537,8 +658,23 @@
       <c r="AO8" s="1"/>
       <c r="AP8" s="1"/>
       <c r="AQ8" s="1"/>
-    </row>
-    <row r="9" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AV8">
+        <v>4.3151562145125215</v>
+      </c>
+      <c r="AX8">
+        <v>4.3145492000507879</v>
+      </c>
+      <c r="AZ8">
+        <v>4.7437911226340193</v>
+      </c>
+      <c r="BB8">
+        <v>4.2568917664147978</v>
+      </c>
+      <c r="BH8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>3.93147181921969</v>
       </c>
@@ -642,8 +778,29 @@
       <c r="AO9" s="1"/>
       <c r="AP9" s="1"/>
       <c r="AQ9" s="1"/>
-    </row>
-    <row r="10" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AU9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AV9">
+        <v>4.1030539582227208</v>
+      </c>
+      <c r="AX9">
+        <v>4.4580286638103868</v>
+      </c>
+      <c r="AZ9">
+        <v>4.1967017749388837</v>
+      </c>
+      <c r="BB9">
+        <v>4.5340149921451269</v>
+      </c>
+      <c r="BH9" t="s">
+        <v>11</v>
+      </c>
+      <c r="BI9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>4.3467761731625796</v>
       </c>
@@ -747,8 +904,36 @@
       <c r="AO10" s="1"/>
       <c r="AP10" s="1"/>
       <c r="AQ10" s="1"/>
-    </row>
-    <row r="11" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AU10" t="s">
+        <v>16</v>
+      </c>
+      <c r="AV10">
+        <f>AV8-AV9</f>
+        <v>0.21210225628980073</v>
+      </c>
+      <c r="AX10">
+        <f t="shared" ref="AW10:BC10" si="2">AX8-AX9</f>
+        <v>-0.14347946375959886</v>
+      </c>
+      <c r="AZ10">
+        <f t="shared" si="2"/>
+        <v>0.54708934769513551</v>
+      </c>
+      <c r="BB10">
+        <f t="shared" si="2"/>
+        <v>-0.2771232257303291</v>
+      </c>
+      <c r="BG10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BH10">
+        <v>4.4580286638103868</v>
+      </c>
+      <c r="BI10">
+        <v>4.4332260376972012</v>
+      </c>
+    </row>
+    <row r="11" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>3.84070547804756</v>
       </c>
@@ -852,44 +1037,102 @@
       <c r="AO11" s="1"/>
       <c r="AP11" s="1"/>
       <c r="AQ11" s="1"/>
-    </row>
-    <row r="12" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AU11" t="s">
+        <v>20</v>
+      </c>
+      <c r="AV11">
+        <f>(AV8/AV9-1)*100</f>
+        <v>5.1693752616813082</v>
+      </c>
+      <c r="AX11">
+        <f t="shared" ref="AW11:BB11" si="3">(AX8/AX9-1)*100</f>
+        <v>-3.2184509023987173</v>
+      </c>
+      <c r="AZ11">
+        <f t="shared" si="3"/>
+        <v>13.036174048919701</v>
+      </c>
+      <c r="BB11">
+        <f t="shared" si="3"/>
+        <v>-6.1120932817916636</v>
+      </c>
+      <c r="BG11" t="s">
+        <v>14</v>
+      </c>
+      <c r="BH11">
+        <v>9.6382647586513492</v>
+      </c>
+      <c r="BI11">
+        <v>9.8018396754248034</v>
+      </c>
+    </row>
+    <row r="12" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF12" t="s">
-        <v>3</v>
-      </c>
-      <c r="AJ12" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK12" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ12" s="2"/>
+      <c r="AK12" s="2"/>
       <c r="AM12" s="2"/>
       <c r="AN12" s="2"/>
       <c r="AO12" s="1"/>
       <c r="AP12" s="1"/>
       <c r="AQ12" s="1"/>
-    </row>
-    <row r="13" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AU12" t="s">
+        <v>1</v>
+      </c>
+      <c r="BG12" t="s">
+        <v>15</v>
+      </c>
+      <c r="BH12">
+        <v>16.216907711420916</v>
+      </c>
+      <c r="BI12">
+        <v>15.944082701894363</v>
+      </c>
+    </row>
+    <row r="13" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF13" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ13" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK13" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>3</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK13" s="2"/>
+      <c r="AL13" t="s">
+        <v>7</v>
       </c>
       <c r="AM13" s="2"/>
-      <c r="AN13" s="2"/>
+      <c r="AN13" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="AO13" s="1"/>
-      <c r="AP13" s="1"/>
+      <c r="AP13" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="AQ13" s="1"/>
-    </row>
-    <row r="14" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AU13" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV13" t="s">
+        <v>6</v>
+      </c>
+      <c r="AX13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AZ13" t="s">
+        <v>8</v>
+      </c>
+      <c r="BB13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>4.5090613181468502</v>
       </c>
@@ -989,31 +1232,42 @@
         <v>0.31818483061429803</v>
       </c>
       <c r="AL14" s="5">
+        <v>4.3902911864138776</v>
+      </c>
+      <c r="AM14" s="2">
+        <v>0.38226562226030902</v>
+      </c>
+      <c r="AN14" s="2">
+        <v>6.9005155587113736</v>
+      </c>
+      <c r="AO14" s="2">
+        <v>1.6944246390510167</v>
+      </c>
+      <c r="AP14" s="2">
+        <v>5.7969225427667022</v>
+      </c>
+      <c r="AQ14" s="2">
+        <v>1.9195844794495021</v>
+      </c>
+      <c r="AR14" s="5"/>
+      <c r="AS14" s="5"/>
+      <c r="AV14">
         <v>4.6606917202296616</v>
       </c>
-      <c r="AM14" s="2">
-        <v>0.31818483061429803</v>
-      </c>
-      <c r="AN14" s="2">
+      <c r="AX14">
         <v>4.3902911864138776</v>
       </c>
-      <c r="AO14" s="2">
-        <v>0.38226562226030902</v>
-      </c>
-      <c r="AP14" s="2">
+      <c r="AZ14">
         <v>6.9005155587113736</v>
       </c>
-      <c r="AQ14" s="2">
-        <v>1.6944246390510167</v>
-      </c>
-      <c r="AR14" s="5">
+      <c r="BB14">
         <v>5.7969225427667022</v>
       </c>
-      <c r="AS14" s="5">
-        <v>1.9195844794495021</v>
-      </c>
-    </row>
-    <row r="15" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="BH14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D15">
         <v>4.07278532196589</v>
       </c>
@@ -1117,8 +1371,26 @@
       <c r="AO15" s="1"/>
       <c r="AP15" s="1"/>
       <c r="AQ15" s="1"/>
-    </row>
-    <row r="16" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AV15">
+        <v>4.2217867287734689</v>
+      </c>
+      <c r="AX15">
+        <v>4.4332260376972012</v>
+      </c>
+      <c r="AZ15">
+        <v>4.3209471511328488</v>
+      </c>
+      <c r="BB15">
+        <v>4.5205202935934148</v>
+      </c>
+      <c r="BH15" t="s">
+        <v>11</v>
+      </c>
+      <c r="BI15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D16">
         <v>6.0428004638458797</v>
       </c>
@@ -1222,8 +1494,33 @@
       <c r="AO16" s="1"/>
       <c r="AP16" s="1"/>
       <c r="AQ16" s="1"/>
-    </row>
-    <row r="17" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AV16">
+        <f>AV14-AV15</f>
+        <v>0.43890499145619266</v>
+      </c>
+      <c r="AX16">
+        <f t="shared" ref="AX16" si="4">AX14-AX15</f>
+        <v>-4.2934851283323638E-2</v>
+      </c>
+      <c r="AZ16">
+        <f t="shared" ref="AZ16" si="5">AZ14-AZ15</f>
+        <v>2.5795684075785248</v>
+      </c>
+      <c r="BB16">
+        <f t="shared" ref="BB16" si="6">BB14-BB15</f>
+        <v>1.2764022491732874</v>
+      </c>
+      <c r="BG16" t="s">
+        <v>13</v>
+      </c>
+      <c r="BH16">
+        <v>4.1967017749388837</v>
+      </c>
+      <c r="BI16">
+        <v>4.3209471511328488</v>
+      </c>
+    </row>
+    <row r="17" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D17">
         <v>5.3331846529911502</v>
       </c>
@@ -1327,44 +1624,102 @@
       <c r="AO17" s="1"/>
       <c r="AP17" s="1"/>
       <c r="AQ17" s="1"/>
-    </row>
-    <row r="18" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AU17" t="s">
+        <v>20</v>
+      </c>
+      <c r="AV17">
+        <f>(AV14/AV15-1)*100</f>
+        <v>10.396190514903282</v>
+      </c>
+      <c r="AX17">
+        <f t="shared" ref="AX17:BB17" si="7">(AX14/AX15-1)*100</f>
+        <v>-0.96847873124975559</v>
+      </c>
+      <c r="AZ17">
+        <f t="shared" si="7"/>
+        <v>59.699142742401378</v>
+      </c>
+      <c r="BB17">
+        <f t="shared" si="7"/>
+        <v>28.235737620340593</v>
+      </c>
+      <c r="BG17" t="s">
+        <v>14</v>
+      </c>
+      <c r="BH17">
+        <v>6.9237412333723753</v>
+      </c>
+      <c r="BI17">
+        <v>7.2199455498044021</v>
+      </c>
+    </row>
+    <row r="18" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF18" t="s">
-        <v>6</v>
-      </c>
-      <c r="AJ18" s="2" t="e">
-        <f t="shared" ref="AJ18:AJ36" si="2">AVERAGE(D18:AG18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK18" s="2" t="e">
-        <f t="shared" ref="AK18:AK36" si="3">_xlfn.STDEV.S(D18:AG18)</f>
-        <v>#DIV/0!</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ18" s="2"/>
+      <c r="AK18" s="2"/>
       <c r="AM18" s="1"/>
       <c r="AN18" s="1"/>
       <c r="AO18" s="1"/>
       <c r="AP18" s="1"/>
       <c r="AQ18" s="1"/>
-    </row>
-    <row r="19" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AU18" t="s">
+        <v>4</v>
+      </c>
+      <c r="BG18" t="s">
+        <v>15</v>
+      </c>
+      <c r="BH18">
+        <v>10.559459629389412</v>
+      </c>
+      <c r="BI18">
+        <v>10.774963435890092</v>
+      </c>
+    </row>
+    <row r="19" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF19" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ19" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK19" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AM19" s="1"/>
-      <c r="AN19" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK19" s="2"/>
+      <c r="AL19" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM19" s="2"/>
+      <c r="AN19" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="AO19" s="1"/>
-      <c r="AP19" s="1"/>
+      <c r="AP19" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="AQ19" s="1"/>
-    </row>
-    <row r="20" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AU19" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV19" t="s">
+        <v>6</v>
+      </c>
+      <c r="AX19" t="s">
+        <v>7</v>
+      </c>
+      <c r="AZ19" t="s">
+        <v>8</v>
+      </c>
+      <c r="BB19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D20">
         <v>7.4555122740376101</v>
       </c>
@@ -1456,11 +1811,11 @@
         <v>7.7585501244283801</v>
       </c>
       <c r="AJ20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="AJ20:AJ35" si="8">AVERAGE(D20:AG20)</f>
         <v>7.0908315304740643</v>
       </c>
       <c r="AK20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="AK20:AK35" si="9">_xlfn.STDEV.S(D20:AG20)</f>
         <v>0.59932276661002337</v>
       </c>
       <c r="AL20" s="5">
@@ -1481,8 +1836,23 @@
       <c r="AQ20" s="2">
         <v>1.1512915599638371</v>
       </c>
-    </row>
-    <row r="21" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AV20">
+        <v>7.0908315304740643</v>
+      </c>
+      <c r="AX20">
+        <v>8.5893338627309852</v>
+      </c>
+      <c r="AZ20">
+        <v>8.0726250323551785</v>
+      </c>
+      <c r="BB20">
+        <v>9.4339768321203703</v>
+      </c>
+      <c r="BH20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D21">
         <v>7.4623693154854198</v>
       </c>
@@ -1574,11 +1944,11 @@
         <v>13.294411021811101</v>
       </c>
       <c r="AJ21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>8.5893338627309852</v>
       </c>
       <c r="AK21" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.7083251276102449</v>
       </c>
       <c r="AL21" s="5"/>
@@ -1587,8 +1957,26 @@
       <c r="AO21" s="2"/>
       <c r="AP21" s="2"/>
       <c r="AQ21" s="2"/>
-    </row>
-    <row r="22" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AV21">
+        <v>6.5052084755275654</v>
+      </c>
+      <c r="AX21">
+        <v>9.6382647586513492</v>
+      </c>
+      <c r="AZ21">
+        <v>6.9237412333723753</v>
+      </c>
+      <c r="BB21">
+        <v>10.126514001709587</v>
+      </c>
+      <c r="BH21" t="s">
+        <v>11</v>
+      </c>
+      <c r="BI21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D22">
         <v>8.2161965336034104</v>
       </c>
@@ -1680,11 +2068,11 @@
         <v>8.2471558472062299</v>
       </c>
       <c r="AJ22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>8.0726250323551785</v>
       </c>
       <c r="AK22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.52762908601412395</v>
       </c>
       <c r="AL22" s="5"/>
@@ -1693,8 +2081,33 @@
       <c r="AO22" s="2"/>
       <c r="AP22" s="2"/>
       <c r="AQ22" s="2"/>
-    </row>
-    <row r="23" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AV22">
+        <f>AV20-AV21</f>
+        <v>0.58562305494649891</v>
+      </c>
+      <c r="AX22">
+        <f t="shared" ref="AX22" si="10">AX20-AX21</f>
+        <v>-1.048930895920364</v>
+      </c>
+      <c r="AZ22">
+        <f t="shared" ref="AZ22" si="11">AZ20-AZ21</f>
+        <v>1.1488837989828031</v>
+      </c>
+      <c r="BB22">
+        <f t="shared" ref="BB22" si="12">BB20-BB21</f>
+        <v>-0.69253716958921707</v>
+      </c>
+      <c r="BG22" t="s">
+        <v>13</v>
+      </c>
+      <c r="BH22">
+        <v>4.1030539582227208</v>
+      </c>
+      <c r="BI22">
+        <v>4.2217867287734689</v>
+      </c>
+    </row>
+    <row r="23" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D23">
         <v>9.7609187895834406</v>
       </c>
@@ -1786,11 +2199,11 @@
         <v>6.9410372941723999</v>
       </c>
       <c r="AJ23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>9.4339768321203703</v>
       </c>
       <c r="AK23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.1512915599638371</v>
       </c>
       <c r="AL23" s="5"/>
@@ -1799,46 +2212,103 @@
       <c r="AO23" s="2"/>
       <c r="AP23" s="2"/>
       <c r="AQ23" s="2"/>
-    </row>
-    <row r="24" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AU23" t="s">
+        <v>20</v>
+      </c>
+      <c r="AV23">
+        <f>(AV20/AV21-1)*100</f>
+        <v>9.002371824816958</v>
+      </c>
+      <c r="AX23">
+        <f t="shared" ref="AX23:BB23" si="13">(AX20/AX21-1)*100</f>
+        <v>-10.882984875247793</v>
+      </c>
+      <c r="AZ23">
+        <f t="shared" si="13"/>
+        <v>16.593395972760973</v>
+      </c>
+      <c r="BB23">
+        <f t="shared" si="13"/>
+        <v>-6.8388506594895482</v>
+      </c>
+      <c r="BG23" t="s">
+        <v>14</v>
+      </c>
+      <c r="BH23">
+        <v>6.5052084755275654</v>
+      </c>
+      <c r="BI23">
+        <v>6.6160894971757473</v>
+      </c>
+    </row>
+    <row r="24" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF24" t="s">
-        <v>6</v>
-      </c>
-      <c r="AJ24" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK24" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="AI24" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ24" s="2"/>
+      <c r="AK24" s="2"/>
       <c r="AL24" s="5"/>
       <c r="AM24" s="2"/>
       <c r="AN24" s="2"/>
       <c r="AO24" s="2"/>
       <c r="AP24" s="2"/>
       <c r="AQ24" s="2"/>
-    </row>
-    <row r="25" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AU24" t="s">
+        <v>4</v>
+      </c>
+      <c r="BG24" t="s">
+        <v>15</v>
+      </c>
+      <c r="BH24">
+        <v>8.5196521018960976</v>
+      </c>
+      <c r="BI24">
+        <v>8.4025380938040506</v>
+      </c>
+    </row>
+    <row r="25" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF25" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ25" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK25" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AL25" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="AI25" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK25" s="2"/>
+      <c r="AL25" t="s">
+        <v>7</v>
+      </c>
       <c r="AM25" s="2"/>
-      <c r="AN25" s="2"/>
-      <c r="AO25" s="2"/>
-      <c r="AP25" s="2"/>
+      <c r="AN25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AO25" s="1"/>
+      <c r="AP25" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="AQ25" s="2"/>
-    </row>
-    <row r="26" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AU25" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV25" t="s">
+        <v>6</v>
+      </c>
+      <c r="AX25" t="s">
+        <v>7</v>
+      </c>
+      <c r="AZ25" t="s">
+        <v>8</v>
+      </c>
+      <c r="BB25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D26">
         <v>7.85702009299</v>
       </c>
@@ -1930,11 +2400,11 @@
         <v>7.9620834761209904</v>
       </c>
       <c r="AJ26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>8.0174685918405455</v>
       </c>
       <c r="AK26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.63282827944364273</v>
       </c>
       <c r="AL26" s="5">
@@ -1955,8 +2425,20 @@
       <c r="AQ26" s="2">
         <v>3.0652320075246342</v>
       </c>
-    </row>
-    <row r="27" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AV26">
+        <v>8.0174685918405455</v>
+      </c>
+      <c r="AX26">
+        <v>8.6190510001893657</v>
+      </c>
+      <c r="AZ26">
+        <v>12.75135957688987</v>
+      </c>
+      <c r="BB26">
+        <v>10.902809543502425</v>
+      </c>
+    </row>
+    <row r="27" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D27">
         <v>6.2422008801175304</v>
       </c>
@@ -2048,11 +2530,11 @@
         <v>6.7048149299311204</v>
       </c>
       <c r="AJ27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>8.6190510001893657</v>
       </c>
       <c r="AK27" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.3132287730918499</v>
       </c>
       <c r="AL27" s="5"/>
@@ -2061,8 +2543,20 @@
       <c r="AO27" s="2"/>
       <c r="AP27" s="2"/>
       <c r="AQ27" s="2"/>
-    </row>
-    <row r="28" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AV27">
+        <v>6.6160894971757473</v>
+      </c>
+      <c r="AX27">
+        <v>9.8018396754248034</v>
+      </c>
+      <c r="AZ27">
+        <v>7.2199455498044021</v>
+      </c>
+      <c r="BB27">
+        <v>10.063961470180555</v>
+      </c>
+    </row>
+    <row r="28" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D28">
         <v>12.0287094898323</v>
       </c>
@@ -2154,11 +2648,11 @@
         <v>20.775179319248</v>
       </c>
       <c r="AJ28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>12.75135957688987</v>
       </c>
       <c r="AK28" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.8940643511753077</v>
       </c>
       <c r="AL28" s="5"/>
@@ -2167,8 +2661,24 @@
       <c r="AO28" s="2"/>
       <c r="AP28" s="2"/>
       <c r="AQ28" s="2"/>
-    </row>
-    <row r="29" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AV28">
+        <f>AV26-AV27</f>
+        <v>1.4013790946647982</v>
+      </c>
+      <c r="AX28">
+        <f t="shared" ref="AX28" si="14">AX26-AX27</f>
+        <v>-1.1827886752354377</v>
+      </c>
+      <c r="AZ28">
+        <f t="shared" ref="AZ28" si="15">AZ26-AZ27</f>
+        <v>5.5314140270854679</v>
+      </c>
+      <c r="BB28">
+        <f t="shared" ref="BB28" si="16">BB26-BB27</f>
+        <v>0.83884807332186995</v>
+      </c>
+    </row>
+    <row r="29" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D29">
         <v>12.2233497883651</v>
       </c>
@@ -2260,11 +2770,11 @@
         <v>9.9048778563608799</v>
       </c>
       <c r="AJ29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>10.902809543502425</v>
       </c>
       <c r="AK29" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>3.0652320075246342</v>
       </c>
       <c r="AL29" s="5"/>
@@ -2273,46 +2783,85 @@
       <c r="AO29" s="2"/>
       <c r="AP29" s="2"/>
       <c r="AQ29" s="2"/>
-    </row>
-    <row r="30" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AU29" t="s">
+        <v>20</v>
+      </c>
+      <c r="AV29">
+        <f>(AV26/AV27-1)*100</f>
+        <v>21.181380561176113</v>
+      </c>
+      <c r="AX29">
+        <f t="shared" ref="AX29:BB29" si="17">(AX26/AX27-1)*100</f>
+        <v>-12.067006953816318</v>
+      </c>
+      <c r="AZ29">
+        <f t="shared" si="17"/>
+        <v>76.612960429255892</v>
+      </c>
+      <c r="BB29">
+        <f t="shared" si="17"/>
+        <v>8.3351677747114827</v>
+      </c>
+    </row>
+    <row r="30" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF30" t="s">
-        <v>7</v>
-      </c>
-      <c r="AJ30" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK30" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="AI30" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ30" s="2"/>
+      <c r="AK30" s="2"/>
       <c r="AL30" s="5"/>
       <c r="AM30" s="2"/>
       <c r="AN30" s="2"/>
       <c r="AO30" s="2"/>
       <c r="AP30" s="2"/>
       <c r="AQ30" s="2"/>
-    </row>
-    <row r="31" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AU30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF31" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ31" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK31" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AL31" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="AI31" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK31" s="2"/>
+      <c r="AL31" t="s">
+        <v>7</v>
+      </c>
       <c r="AM31" s="2"/>
-      <c r="AN31" s="2"/>
-      <c r="AO31" s="2"/>
-      <c r="AP31" s="2"/>
+      <c r="AN31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AO31" s="1"/>
+      <c r="AP31" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="AQ31" s="2"/>
-    </row>
-    <row r="32" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AU31" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV31" t="s">
+        <v>6</v>
+      </c>
+      <c r="AX31" t="s">
+        <v>7</v>
+      </c>
+      <c r="AZ31" t="s">
+        <v>8</v>
+      </c>
+      <c r="BB31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D32">
         <v>9.14871860127659</v>
       </c>
@@ -2404,11 +2953,11 @@
         <v>8.9292585727315803</v>
       </c>
       <c r="AJ32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>9.3416814204142913</v>
       </c>
       <c r="AK32" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.110498757620775</v>
       </c>
       <c r="AL32" s="5">
@@ -2429,8 +2978,20 @@
       <c r="AQ32" s="2">
         <v>2.7167443958416784</v>
       </c>
-    </row>
-    <row r="33" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AV32">
+        <v>9.3416814204142913</v>
+      </c>
+      <c r="AX32">
+        <v>15.374403149212615</v>
+      </c>
+      <c r="AZ32">
+        <v>12.664070588477017</v>
+      </c>
+      <c r="BB32">
+        <v>18.711215843700355</v>
+      </c>
+    </row>
+    <row r="33" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D33">
         <v>16.541181728659499</v>
       </c>
@@ -2522,11 +3083,11 @@
         <v>15.7100907331368</v>
       </c>
       <c r="AJ33" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>15.374403149212615</v>
       </c>
       <c r="AK33" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.5991176303019512</v>
       </c>
       <c r="AL33" s="5"/>
@@ -2535,8 +3096,20 @@
       <c r="AO33" s="2"/>
       <c r="AP33" s="2"/>
       <c r="AQ33" s="2"/>
-    </row>
-    <row r="34" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AV33">
+        <v>8.5196521018960976</v>
+      </c>
+      <c r="AX33">
+        <v>16.216907711420916</v>
+      </c>
+      <c r="AZ33">
+        <v>10.559459629389412</v>
+      </c>
+      <c r="BB33">
+        <v>19.104781491799571</v>
+      </c>
+    </row>
+    <row r="34" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D34">
         <v>10.9660527770196</v>
       </c>
@@ -2628,11 +3201,11 @@
         <v>12.7889528948216</v>
       </c>
       <c r="AJ34" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>12.664070588477017</v>
       </c>
       <c r="AK34" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.1907723989377514</v>
       </c>
       <c r="AL34" s="5"/>
@@ -2641,8 +3214,24 @@
       <c r="AO34" s="2"/>
       <c r="AP34" s="2"/>
       <c r="AQ34" s="2"/>
-    </row>
-    <row r="35" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AV34">
+        <f>AV32-AV33</f>
+        <v>0.82202931851819372</v>
+      </c>
+      <c r="AX34">
+        <f t="shared" ref="AX34" si="18">AX32-AX33</f>
+        <v>-0.84250456220830117</v>
+      </c>
+      <c r="AZ34">
+        <f t="shared" ref="AZ34" si="19">AZ32-AZ33</f>
+        <v>2.104610959087605</v>
+      </c>
+      <c r="BB34">
+        <f t="shared" ref="BB34" si="20">BB32-BB33</f>
+        <v>-0.39356564809921579</v>
+      </c>
+    </row>
+    <row r="35" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D35">
         <v>19.640271484319602</v>
       </c>
@@ -2734,11 +3323,11 @@
         <v>22.189920552475201</v>
       </c>
       <c r="AJ35" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>18.711215843700355</v>
       </c>
       <c r="AK35" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.7167443958416784</v>
       </c>
       <c r="AL35" s="5"/>
@@ -2747,46 +3336,85 @@
       <c r="AO35" s="2"/>
       <c r="AP35" s="2"/>
       <c r="AQ35" s="2"/>
-    </row>
-    <row r="36" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AU35" t="s">
+        <v>20</v>
+      </c>
+      <c r="AV35">
+        <f>(AV32/AV33-1)*100</f>
+        <v>9.6486254213977496</v>
+      </c>
+      <c r="AX35">
+        <f t="shared" ref="AX35:BB35" si="21">(AX32/AX33-1)*100</f>
+        <v>-5.1952232645127499</v>
+      </c>
+      <c r="AZ35">
+        <f t="shared" si="21"/>
+        <v>19.931047922471222</v>
+      </c>
+      <c r="BB35">
+        <f t="shared" si="21"/>
+        <v>-2.0600374218786466</v>
+      </c>
+    </row>
+    <row r="36" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF36" t="s">
-        <v>7</v>
-      </c>
-      <c r="AJ36" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK36" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="AI36" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ36" s="2"/>
+      <c r="AK36" s="2"/>
       <c r="AL36" s="5"/>
       <c r="AM36" s="2"/>
       <c r="AN36" s="2"/>
       <c r="AO36" s="2"/>
       <c r="AP36" s="2"/>
       <c r="AQ36" s="2"/>
-    </row>
-    <row r="37" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AU36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF37" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ37" s="2" t="e">
-        <f t="shared" ref="AJ37:AJ77" si="4">AVERAGE(D37:AG37)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK37" s="2" t="e">
-        <f t="shared" ref="AK37:AK77" si="5">_xlfn.STDEV.S(D37:AG37)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AL37" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="AI37" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK37" s="2"/>
+      <c r="AL37" t="s">
+        <v>7</v>
+      </c>
       <c r="AM37" s="2"/>
-      <c r="AN37" s="2"/>
-      <c r="AO37" s="2"/>
-      <c r="AP37" s="2"/>
+      <c r="AN37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AO37" s="1"/>
+      <c r="AP37" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="AQ37" s="2"/>
-    </row>
-    <row r="38" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AU37" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV37" t="s">
+        <v>6</v>
+      </c>
+      <c r="AX37" t="s">
+        <v>7</v>
+      </c>
+      <c r="AZ37" t="s">
+        <v>8</v>
+      </c>
+      <c r="BB37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D38">
         <v>12.186678730118</v>
       </c>
@@ -2878,11 +3506,11 @@
         <v>12.708205534623</v>
       </c>
       <c r="AJ38" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="AJ38:AJ41" si="22">AVERAGE(D38:AG38)</f>
         <v>12.186117717401205</v>
       </c>
       <c r="AK38" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="AK38:AK41" si="23">_xlfn.STDEV.S(D38:AG38)</f>
         <v>1.5543448361996259</v>
       </c>
       <c r="AL38" s="2">
@@ -2903,8 +3531,20 @@
       <c r="AQ38" s="2">
         <v>11.021409584412559</v>
       </c>
-    </row>
-    <row r="39" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AV38">
+        <v>12.186117717401205</v>
+      </c>
+      <c r="AX38">
+        <v>16.987513012340507</v>
+      </c>
+      <c r="AZ38">
+        <v>23.38056567610445</v>
+      </c>
+      <c r="BB38">
+        <v>29.32912838340696</v>
+      </c>
+    </row>
+    <row r="39" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D39">
         <v>20.4091701925243</v>
       </c>
@@ -2996,11 +3636,11 @@
         <v>12.0706517018996</v>
       </c>
       <c r="AJ39" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="22"/>
         <v>16.987513012340507</v>
       </c>
       <c r="AK39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="23"/>
         <v>3.8142685872044444</v>
       </c>
       <c r="AM39" s="2"/>
@@ -3008,8 +3648,20 @@
       <c r="AO39" s="1"/>
       <c r="AP39" s="1"/>
       <c r="AQ39" s="1"/>
-    </row>
-    <row r="40" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AV39">
+        <v>8.4025380938040506</v>
+      </c>
+      <c r="AX39">
+        <v>15.944082701894363</v>
+      </c>
+      <c r="AZ39">
+        <v>10.774963435890092</v>
+      </c>
+      <c r="BB39">
+        <v>18.904530166296727</v>
+      </c>
+    </row>
+    <row r="40" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D40">
         <v>29.3160265856596</v>
       </c>
@@ -3101,11 +3753,11 @@
         <v>33.075049130053699</v>
       </c>
       <c r="AJ40" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="22"/>
         <v>23.38056567610445</v>
       </c>
       <c r="AK40" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="23"/>
         <v>5.4029592432716465</v>
       </c>
       <c r="AM40" s="2"/>
@@ -3113,8 +3765,24 @@
       <c r="AO40" s="1"/>
       <c r="AP40" s="1"/>
       <c r="AQ40" s="1"/>
-    </row>
-    <row r="41" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AV40">
+        <f>AV38-AV39</f>
+        <v>3.7835796235971539</v>
+      </c>
+      <c r="AX40">
+        <f t="shared" ref="AX40" si="24">AX38-AX39</f>
+        <v>1.0434303104461442</v>
+      </c>
+      <c r="AZ40">
+        <f t="shared" ref="AZ40" si="25">AZ38-AZ39</f>
+        <v>12.605602240214358</v>
+      </c>
+      <c r="BB40">
+        <f t="shared" ref="BB40" si="26">BB38-BB39</f>
+        <v>10.424598217110233</v>
+      </c>
+    </row>
+    <row r="41" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D41">
         <v>21.7314376586049</v>
       </c>
@@ -3206,11 +3874,11 @@
         <v>52.991459776885399</v>
       </c>
       <c r="AJ41" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="22"/>
         <v>29.32912838340696</v>
       </c>
       <c r="AK41" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="23"/>
         <v>11.021409584412559</v>
       </c>
       <c r="AM41" s="2"/>
@@ -3218,106 +3886,83 @@
       <c r="AO41" s="1"/>
       <c r="AP41" s="1"/>
       <c r="AQ41" s="1"/>
-    </row>
-    <row r="42" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ42" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK42" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AU41" t="s">
+        <v>20</v>
+      </c>
+      <c r="AV41">
+        <f>(AV38/AV39-1)*100</f>
+        <v>45.029008870392715</v>
+      </c>
+      <c r="AX41">
+        <f t="shared" ref="AX41:BB41" si="27">(AX38/AX39-1)*100</f>
+        <v>6.5443107010613399</v>
+      </c>
+      <c r="AZ41">
+        <f t="shared" si="27"/>
+        <v>116.98974493246661</v>
+      </c>
+      <c r="BB41">
+        <f t="shared" si="27"/>
+        <v>55.143386931114314</v>
+      </c>
+    </row>
+    <row r="42" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AJ42" s="2"/>
+      <c r="AK42" s="2"/>
       <c r="AM42" s="2"/>
       <c r="AN42" s="2"/>
       <c r="AO42" s="1"/>
       <c r="AP42" s="1"/>
       <c r="AQ42" s="1"/>
     </row>
-    <row r="43" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ43" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK43" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+    <row r="43" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AJ43" s="2"/>
+      <c r="AK43" s="2"/>
       <c r="AM43" s="1"/>
       <c r="AN43" s="2"/>
       <c r="AO43" s="1"/>
       <c r="AP43" s="1"/>
       <c r="AQ43" s="1"/>
     </row>
-    <row r="44" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ44" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK44" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+    <row r="44" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AJ44" s="2"/>
+      <c r="AK44" s="2"/>
       <c r="AM44" s="1"/>
       <c r="AN44" s="2"/>
       <c r="AO44" s="1"/>
       <c r="AP44" s="1"/>
       <c r="AQ44" s="1"/>
     </row>
-    <row r="45" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ45" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK45" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+    <row r="45" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AJ45" s="2"/>
+      <c r="AK45" s="2"/>
       <c r="AM45" s="2"/>
       <c r="AN45" s="2"/>
       <c r="AO45" s="1"/>
       <c r="AP45" s="1"/>
       <c r="AQ45" s="1"/>
     </row>
-    <row r="46" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ46" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK46" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+    <row r="46" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AJ46" s="2"/>
+      <c r="AK46" s="2"/>
       <c r="AM46" s="2"/>
       <c r="AN46" s="2"/>
       <c r="AO46" s="1"/>
       <c r="AP46" s="1"/>
       <c r="AQ46" s="1"/>
     </row>
-    <row r="47" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ47" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK47" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+    <row r="47" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AJ47" s="2"/>
+      <c r="AK47" s="2"/>
       <c r="AM47" s="2"/>
       <c r="AN47" s="2"/>
       <c r="AO47" s="1"/>
       <c r="AP47" s="1"/>
       <c r="AQ47" s="1"/>
     </row>
-    <row r="48" spans="4:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ48" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK48" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+    <row r="48" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AJ48" s="2"/>
+      <c r="AK48" s="2"/>
       <c r="AM48" s="2"/>
       <c r="AN48" s="1"/>
       <c r="AO48" s="1"/>
@@ -3325,14 +3970,8 @@
       <c r="AQ48" s="1"/>
     </row>
     <row r="49" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ49" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK49" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ49" s="2"/>
+      <c r="AK49" s="2"/>
       <c r="AM49" s="1"/>
       <c r="AN49" s="1"/>
       <c r="AO49" s="1"/>
@@ -3340,14 +3979,8 @@
       <c r="AQ49" s="1"/>
     </row>
     <row r="50" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ50" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK50" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ50" s="2"/>
+      <c r="AK50" s="2"/>
       <c r="AM50" s="2"/>
       <c r="AN50" s="2"/>
       <c r="AO50" s="1"/>
@@ -3355,14 +3988,8 @@
       <c r="AQ50" s="1"/>
     </row>
     <row r="51" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ51" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK51" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ51" s="2"/>
+      <c r="AK51" s="2"/>
       <c r="AM51" s="2"/>
       <c r="AN51" s="2"/>
       <c r="AO51" s="1"/>
@@ -3370,14 +3997,8 @@
       <c r="AQ51" s="1"/>
     </row>
     <row r="52" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ52" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK52" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ52" s="2"/>
+      <c r="AK52" s="2"/>
       <c r="AM52" s="1"/>
       <c r="AN52" s="1"/>
       <c r="AO52" s="1"/>
@@ -3385,14 +4006,8 @@
       <c r="AQ52" s="1"/>
     </row>
     <row r="53" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ53" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK53" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ53" s="2"/>
+      <c r="AK53" s="2"/>
       <c r="AM53" s="2"/>
       <c r="AN53" s="1"/>
       <c r="AO53" s="1"/>
@@ -3401,14 +4016,8 @@
     </row>
     <row r="54" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF54" s="4"/>
-      <c r="AJ54" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK54" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ54" s="2"/>
+      <c r="AK54" s="2"/>
       <c r="AM54" s="2"/>
       <c r="AN54" s="1"/>
       <c r="AO54" s="1"/>
@@ -3416,14 +4025,8 @@
       <c r="AQ54" s="1"/>
     </row>
     <row r="55" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ55" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK55" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ55" s="2"/>
+      <c r="AK55" s="2"/>
       <c r="AM55" s="2"/>
       <c r="AN55" s="2"/>
       <c r="AO55" s="1"/>
@@ -3431,14 +4034,8 @@
       <c r="AQ55" s="1"/>
     </row>
     <row r="56" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ56" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK56" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ56" s="2"/>
+      <c r="AK56" s="2"/>
       <c r="AM56" s="2"/>
       <c r="AN56" s="2"/>
       <c r="AO56" s="1"/>
@@ -3446,14 +4043,8 @@
       <c r="AQ56" s="1"/>
     </row>
     <row r="57" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ57" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK57" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ57" s="2"/>
+      <c r="AK57" s="2"/>
       <c r="AM57" s="1"/>
       <c r="AN57" s="1"/>
       <c r="AO57" s="1"/>
@@ -3461,14 +4052,8 @@
       <c r="AQ57" s="1"/>
     </row>
     <row r="58" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ58" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK58" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ58" s="2"/>
+      <c r="AK58" s="2"/>
       <c r="AM58" s="1"/>
       <c r="AN58" s="1"/>
       <c r="AO58" s="1"/>
@@ -3476,14 +4061,8 @@
       <c r="AQ58" s="1"/>
     </row>
     <row r="59" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ59" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK59" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ59" s="2"/>
+      <c r="AK59" s="2"/>
       <c r="AM59" s="2"/>
       <c r="AN59" s="2"/>
       <c r="AO59" s="1"/>
@@ -3491,14 +4070,8 @@
       <c r="AQ59" s="1"/>
     </row>
     <row r="60" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ60" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK60" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ60" s="2"/>
+      <c r="AK60" s="2"/>
       <c r="AM60" s="2"/>
       <c r="AN60" s="2"/>
       <c r="AO60" s="1"/>
@@ -3506,14 +4079,8 @@
       <c r="AQ60" s="1"/>
     </row>
     <row r="61" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ61" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK61" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ61" s="2"/>
+      <c r="AK61" s="2"/>
       <c r="AM61" s="2"/>
       <c r="AN61" s="2"/>
       <c r="AO61" s="1"/>
@@ -3521,14 +4088,8 @@
       <c r="AQ61" s="1"/>
     </row>
     <row r="62" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ62" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK62" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ62" s="2"/>
+      <c r="AK62" s="2"/>
       <c r="AM62" s="2"/>
       <c r="AN62" s="2"/>
       <c r="AO62" s="1"/>
@@ -3536,14 +4097,8 @@
       <c r="AQ62" s="1"/>
     </row>
     <row r="63" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ63" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK63" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ63" s="2"/>
+      <c r="AK63" s="2"/>
       <c r="AM63" s="1"/>
       <c r="AN63" s="1"/>
       <c r="AO63" s="1"/>
@@ -3551,14 +4106,8 @@
       <c r="AQ63" s="1"/>
     </row>
     <row r="64" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ64" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK64" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ64" s="2"/>
+      <c r="AK64" s="2"/>
       <c r="AM64" s="2"/>
       <c r="AN64" s="2"/>
       <c r="AO64" s="1"/>
@@ -3566,14 +4115,8 @@
       <c r="AQ64" s="1"/>
     </row>
     <row r="65" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ65" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK65" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ65" s="2"/>
+      <c r="AK65" s="2"/>
       <c r="AM65" s="2"/>
       <c r="AN65" s="2"/>
       <c r="AO65" s="1"/>
@@ -3582,14 +4125,8 @@
     </row>
     <row r="66" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF66" s="4"/>
-      <c r="AJ66" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK66" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ66" s="2"/>
+      <c r="AK66" s="2"/>
       <c r="AM66" s="1"/>
       <c r="AN66" s="1"/>
       <c r="AO66" s="1"/>
@@ -3597,14 +4134,8 @@
       <c r="AQ66" s="1"/>
     </row>
     <row r="67" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ67" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK67" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ67" s="2"/>
+      <c r="AK67" s="2"/>
       <c r="AM67" s="1"/>
       <c r="AN67" s="1"/>
       <c r="AO67" s="1"/>
@@ -3612,14 +4143,8 @@
       <c r="AQ67" s="1"/>
     </row>
     <row r="68" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ68" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK68" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ68" s="2"/>
+      <c r="AK68" s="2"/>
       <c r="AM68" s="1"/>
       <c r="AN68" s="1"/>
       <c r="AO68" s="1"/>
@@ -3627,14 +4152,8 @@
       <c r="AQ68" s="1"/>
     </row>
     <row r="69" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ69" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK69" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ69" s="2"/>
+      <c r="AK69" s="2"/>
       <c r="AM69" s="1"/>
       <c r="AN69" s="1"/>
       <c r="AO69" s="1"/>
@@ -3642,14 +4161,8 @@
       <c r="AQ69" s="1"/>
     </row>
     <row r="70" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ70" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK70" s="2" t="e">
-        <f>_xlfn.STDEV.S(D70:AG70)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ70" s="2"/>
+      <c r="AK70" s="2"/>
       <c r="AM70" s="1"/>
       <c r="AN70" s="1"/>
       <c r="AO70" s="1"/>
@@ -3657,14 +4170,8 @@
       <c r="AQ70" s="1"/>
     </row>
     <row r="71" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ71" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK71" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ71" s="2"/>
+      <c r="AK71" s="2"/>
       <c r="AM71" s="1"/>
       <c r="AN71" s="1"/>
       <c r="AO71" s="1"/>
@@ -3672,14 +4179,8 @@
       <c r="AQ71" s="1"/>
     </row>
     <row r="72" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ72" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK72" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ72" s="2"/>
+      <c r="AK72" s="2"/>
       <c r="AM72" s="1"/>
       <c r="AN72" s="1"/>
       <c r="AO72" s="1"/>
@@ -3687,14 +4188,8 @@
       <c r="AQ72" s="1"/>
     </row>
     <row r="73" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ73" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK73" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ73" s="2"/>
+      <c r="AK73" s="2"/>
       <c r="AM73" s="1"/>
       <c r="AN73" s="1"/>
       <c r="AO73" s="1"/>
@@ -3702,14 +4197,8 @@
       <c r="AQ73" s="1"/>
     </row>
     <row r="74" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ74" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK74" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ74" s="2"/>
+      <c r="AK74" s="2"/>
       <c r="AM74" s="2"/>
       <c r="AN74" s="2"/>
       <c r="AO74" s="1"/>
@@ -3717,14 +4206,8 @@
       <c r="AQ74" s="1"/>
     </row>
     <row r="75" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ75" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK75" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ75" s="2"/>
+      <c r="AK75" s="2"/>
       <c r="AM75" s="2"/>
       <c r="AN75" s="2"/>
       <c r="AO75" s="1"/>
@@ -3732,14 +4215,8 @@
       <c r="AQ75" s="1"/>
     </row>
     <row r="76" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ76" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK76" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ76" s="2"/>
+      <c r="AK76" s="2"/>
       <c r="AM76" s="2"/>
       <c r="AN76" s="2"/>
       <c r="AO76" s="1"/>
@@ -3747,14 +4224,8 @@
       <c r="AQ76" s="1"/>
     </row>
     <row r="77" spans="32:43" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AJ77" s="2" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK77" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ77" s="2"/>
+      <c r="AK77" s="2"/>
       <c r="AM77" s="2"/>
       <c r="AN77" s="2"/>
       <c r="AO77" s="1"/>

</xml_diff>

<commit_message>
Acabado el caso de estudio 5
</commit_message>
<xml_diff>
--- a/Proyecto/Caso5.xlsx
+++ b/Proyecto/Caso5.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="9975" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="9975" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja 1" sheetId="4" r:id="rId1"/>
+    <sheet name="1 cluster" sheetId="4" r:id="rId1"/>
+    <sheet name="2 clusters" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="30">
   <si>
     <t>Clusters 1</t>
   </si>
@@ -46,9 +47,6 @@
     <t>Caso 4</t>
   </si>
   <si>
-    <t>Comparacion</t>
-  </si>
-  <si>
     <t>Iso</t>
   </si>
   <si>
@@ -64,9 +62,6 @@
     <t>20 sensores</t>
   </si>
   <si>
-    <t>Mejora</t>
-  </si>
-  <si>
     <t>Caso4</t>
   </si>
   <si>
@@ -77,6 +72,39 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>Caso5</t>
+  </si>
+  <si>
+    <t>Diferencia</t>
+  </si>
+  <si>
+    <t>5 sensores iso</t>
+  </si>
+  <si>
+    <t>5 sensores dip</t>
+  </si>
+  <si>
+    <t>10 sensores iso</t>
+  </si>
+  <si>
+    <t>10 sensores dip</t>
+  </si>
+  <si>
+    <t>20 sensores iso</t>
+  </si>
+  <si>
+    <t>20 sensores dip</t>
+  </si>
+  <si>
+    <t>isotropica</t>
+  </si>
+  <si>
+    <t>Caso 1</t>
+  </si>
+  <si>
+    <t>dipolo</t>
   </si>
 </sst>
 </file>
@@ -122,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -135,6 +163,9 @@
     </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:BI91"/>
+  <dimension ref="D2:BL91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AU41" sqref="AU41:BB41"/>
+    <sheetView topLeftCell="AT1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AV9" sqref="AV9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,44 +484,48 @@
     <col min="44" max="44" width="13" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="17.5703125" customWidth="1"/>
+    <col min="48" max="49" width="20" bestFit="1" customWidth="1"/>
+    <col min="50" max="51" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:61" x14ac:dyDescent="0.25">
-      <c r="BH2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="4:61" x14ac:dyDescent="0.25">
-      <c r="BH3" t="s">
+    <row r="2" spans="4:64" x14ac:dyDescent="0.25">
+      <c r="BK2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="4:64" x14ac:dyDescent="0.25">
+      <c r="BK3" t="s">
+        <v>10</v>
+      </c>
+      <c r="BL3" t="s">
         <v>11</v>
       </c>
-      <c r="BI3" t="s">
+    </row>
+    <row r="4" spans="4:64" x14ac:dyDescent="0.25">
+      <c r="BJ4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="4:61" x14ac:dyDescent="0.25">
-      <c r="BG4" t="s">
+      <c r="BK4">
+        <v>4.5340149921451269</v>
+      </c>
+      <c r="BL4">
+        <v>4.5205202935934148</v>
+      </c>
+    </row>
+    <row r="5" spans="4:64" x14ac:dyDescent="0.25">
+      <c r="BJ5" t="s">
         <v>13</v>
       </c>
-      <c r="BH4">
-        <v>4.5340149921451269</v>
-      </c>
-      <c r="BI4">
-        <v>4.5205202935934148</v>
-      </c>
-    </row>
-    <row r="5" spans="4:61" x14ac:dyDescent="0.25">
-      <c r="BG5" t="s">
-        <v>14</v>
-      </c>
-      <c r="BH5">
+      <c r="BK5">
         <v>10.126514001709587</v>
       </c>
-      <c r="BI5">
+      <c r="BL5">
         <v>10.063961470180555</v>
       </c>
     </row>
-    <row r="6" spans="4:61" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:64" x14ac:dyDescent="0.25">
       <c r="AF6" t="s">
         <v>1</v>
       </c>
@@ -500,23 +535,17 @@
       <c r="AJ6" t="s">
         <v>0</v>
       </c>
-      <c r="AU6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AV6" t="s">
-        <v>0</v>
-      </c>
-      <c r="BG6" t="s">
-        <v>15</v>
-      </c>
-      <c r="BH6">
+      <c r="BJ6" t="s">
+        <v>14</v>
+      </c>
+      <c r="BK6">
         <v>19.104781491799571</v>
       </c>
-      <c r="BI6">
+      <c r="BL6">
         <v>18.904530166296727</v>
       </c>
     </row>
-    <row r="7" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF7" t="s">
         <v>2</v>
       </c>
@@ -538,23 +567,29 @@
       <c r="AP7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AU7" t="s">
-        <v>2</v>
-      </c>
       <c r="AV7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AW7" t="s">
         <v>6</v>
       </c>
       <c r="AX7" t="s">
+        <v>20</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>18</v>
+      </c>
+      <c r="BE7" t="s">
         <v>7</v>
       </c>
-      <c r="AZ7" t="s">
+      <c r="BG7" t="s">
         <v>8</v>
       </c>
-      <c r="BB7" t="s">
+      <c r="BI7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>4.1397369554959296</v>
       </c>
@@ -658,23 +693,37 @@
       <c r="AO8" s="1"/>
       <c r="AP8" s="1"/>
       <c r="AQ8" s="1"/>
-      <c r="AV8">
+      <c r="AU8" t="s">
+        <v>21</v>
+      </c>
+      <c r="AV8" s="6">
         <v>4.3151562145125215</v>
       </c>
-      <c r="AX8">
+      <c r="AW8" s="6">
+        <v>4.1030539582227208</v>
+      </c>
+      <c r="AX8" s="6">
+        <f>AV8-AW8</f>
+        <v>0.21210225628980073</v>
+      </c>
+      <c r="AY8" s="6">
+        <f>(AV8/AW8-1)*100</f>
+        <v>5.1693752616813082</v>
+      </c>
+      <c r="BE8">
         <v>4.3145492000507879</v>
       </c>
-      <c r="AZ8">
+      <c r="BG8">
         <v>4.7437911226340193</v>
       </c>
-      <c r="BB8">
+      <c r="BI8">
         <v>4.2568917664147978</v>
       </c>
-      <c r="BH8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="BK8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>3.93147181921969</v>
       </c>
@@ -779,28 +828,39 @@
       <c r="AP9" s="1"/>
       <c r="AQ9" s="1"/>
       <c r="AU9" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV9" s="6">
+        <v>4.6606917202296616</v>
+      </c>
+      <c r="AW9" s="6">
+        <v>4.2217867287734689</v>
+      </c>
+      <c r="AX9" s="6">
+        <f>AV9-AW9</f>
+        <v>0.43890499145619266</v>
+      </c>
+      <c r="AY9" s="6">
+        <f>(AV9/AW9-1)*100</f>
+        <v>10.396190514903282</v>
+      </c>
+      <c r="BE9">
+        <v>4.4580286638103868</v>
+      </c>
+      <c r="BG9">
+        <v>4.1967017749388837</v>
+      </c>
+      <c r="BI9">
+        <v>4.5340149921451269</v>
+      </c>
+      <c r="BK9" t="s">
         <v>10</v>
       </c>
-      <c r="AV9">
-        <v>4.1030539582227208</v>
-      </c>
-      <c r="AX9">
-        <v>4.4580286638103868</v>
-      </c>
-      <c r="AZ9">
-        <v>4.1967017749388837</v>
-      </c>
-      <c r="BB9">
-        <v>4.5340149921451269</v>
-      </c>
-      <c r="BH9" t="s">
+      <c r="BL9" t="s">
         <v>11</v>
       </c>
-      <c r="BI9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>4.3467761731625796</v>
       </c>
@@ -905,35 +965,45 @@
       <c r="AP10" s="1"/>
       <c r="AQ10" s="1"/>
       <c r="AU10" t="s">
-        <v>16</v>
-      </c>
-      <c r="AV10">
-        <f>AV8-AV9</f>
-        <v>0.21210225628980073</v>
-      </c>
-      <c r="AX10">
-        <f t="shared" ref="AW10:BC10" si="2">AX8-AX9</f>
+        <v>23</v>
+      </c>
+      <c r="AV10" s="6">
+        <v>7.0908315304740643</v>
+      </c>
+      <c r="AW10" s="6">
+        <v>6.5052084755275654</v>
+      </c>
+      <c r="AX10" s="6">
+        <f>AV10-AW10</f>
+        <v>0.58562305494649891</v>
+      </c>
+      <c r="AY10" s="6">
+        <f>(AV10/AW10-1)*100</f>
+        <v>9.002371824816958</v>
+      </c>
+      <c r="BE10">
+        <f t="shared" ref="BE10:BI10" si="2">BE8-BE9</f>
         <v>-0.14347946375959886</v>
       </c>
-      <c r="AZ10">
+      <c r="BG10">
         <f t="shared" si="2"/>
         <v>0.54708934769513551</v>
       </c>
-      <c r="BB10">
+      <c r="BI10">
         <f t="shared" si="2"/>
         <v>-0.2771232257303291</v>
       </c>
-      <c r="BG10" t="s">
-        <v>13</v>
-      </c>
-      <c r="BH10">
+      <c r="BJ10" t="s">
+        <v>12</v>
+      </c>
+      <c r="BK10">
         <v>4.4580286638103868</v>
       </c>
-      <c r="BI10">
+      <c r="BL10">
         <v>4.4332260376972012</v>
       </c>
     </row>
-    <row r="11" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>3.84070547804756</v>
       </c>
@@ -1038,35 +1108,45 @@
       <c r="AP11" s="1"/>
       <c r="AQ11" s="1"/>
       <c r="AU11" t="s">
-        <v>20</v>
-      </c>
-      <c r="AV11">
-        <f>(AV8/AV9-1)*100</f>
-        <v>5.1693752616813082</v>
-      </c>
-      <c r="AX11">
-        <f t="shared" ref="AW11:BB11" si="3">(AX8/AX9-1)*100</f>
+        <v>24</v>
+      </c>
+      <c r="AV11" s="6">
+        <v>8.0174685918405455</v>
+      </c>
+      <c r="AW11" s="6">
+        <v>6.6160894971757473</v>
+      </c>
+      <c r="AX11" s="6">
+        <f>AV11-AW11</f>
+        <v>1.4013790946647982</v>
+      </c>
+      <c r="AY11" s="6">
+        <f>(AV11/AW11-1)*100</f>
+        <v>21.181380561176113</v>
+      </c>
+      <c r="BE11">
+        <f t="shared" ref="BE11:BI11" si="3">(BE8/BE9-1)*100</f>
         <v>-3.2184509023987173</v>
       </c>
-      <c r="AZ11">
+      <c r="BG11">
         <f t="shared" si="3"/>
         <v>13.036174048919701</v>
       </c>
-      <c r="BB11">
+      <c r="BI11">
         <f t="shared" si="3"/>
         <v>-6.1120932817916636</v>
       </c>
-      <c r="BG11" t="s">
-        <v>14</v>
-      </c>
-      <c r="BH11">
+      <c r="BJ11" t="s">
+        <v>13</v>
+      </c>
+      <c r="BK11">
         <v>9.6382647586513492</v>
       </c>
-      <c r="BI11">
+      <c r="BL11">
         <v>9.8018396754248034</v>
       </c>
     </row>
-    <row r="12" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF12" t="s">
         <v>1</v>
       </c>
@@ -1081,19 +1161,33 @@
       <c r="AP12" s="1"/>
       <c r="AQ12" s="1"/>
       <c r="AU12" t="s">
-        <v>1</v>
-      </c>
-      <c r="BG12" t="s">
-        <v>15</v>
-      </c>
-      <c r="BH12">
+        <v>25</v>
+      </c>
+      <c r="AV12" s="6">
+        <v>9.3416814204142913</v>
+      </c>
+      <c r="AW12" s="6">
+        <v>8.5196521018960976</v>
+      </c>
+      <c r="AX12" s="6">
+        <f>AV12-AW12</f>
+        <v>0.82202931851819372</v>
+      </c>
+      <c r="AY12" s="6">
+        <f>(AV12/AW12-1)*100</f>
+        <v>9.6486254213977496</v>
+      </c>
+      <c r="BJ12" t="s">
+        <v>14</v>
+      </c>
+      <c r="BK12">
         <v>16.216907711420916</v>
       </c>
-      <c r="BI12">
+      <c r="BL12">
         <v>15.944082701894363</v>
       </c>
     </row>
-    <row r="13" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF13" t="s">
         <v>3</v>
       </c>
@@ -1117,22 +1211,33 @@
       </c>
       <c r="AQ13" s="1"/>
       <c r="AU13" t="s">
-        <v>3</v>
-      </c>
-      <c r="AV13" t="s">
-        <v>6</v>
-      </c>
-      <c r="AX13" t="s">
+        <v>26</v>
+      </c>
+      <c r="AV13" s="6">
+        <v>12.186117717401205</v>
+      </c>
+      <c r="AW13" s="6">
+        <v>8.4025380938040506</v>
+      </c>
+      <c r="AX13" s="6">
+        <f>AV13-AW13</f>
+        <v>3.7835796235971539</v>
+      </c>
+      <c r="AY13" s="6">
+        <f>(AV13/AW13-1)*100</f>
+        <v>45.029008870392715</v>
+      </c>
+      <c r="BE13" t="s">
         <v>7</v>
       </c>
-      <c r="AZ13" t="s">
+      <c r="BG13" t="s">
         <v>8</v>
       </c>
-      <c r="BB13" t="s">
+      <c r="BI13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>4.5090613181468502</v>
       </c>
@@ -1251,23 +1356,20 @@
       </c>
       <c r="AR14" s="5"/>
       <c r="AS14" s="5"/>
-      <c r="AV14">
-        <v>4.6606917202296616</v>
-      </c>
-      <c r="AX14">
+      <c r="BE14">
         <v>4.3902911864138776</v>
       </c>
-      <c r="AZ14">
+      <c r="BG14">
         <v>6.9005155587113736</v>
       </c>
-      <c r="BB14">
+      <c r="BI14">
         <v>5.7969225427667022</v>
       </c>
-      <c r="BH14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="BK14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D15">
         <v>4.07278532196589</v>
       </c>
@@ -1371,26 +1473,23 @@
       <c r="AO15" s="1"/>
       <c r="AP15" s="1"/>
       <c r="AQ15" s="1"/>
-      <c r="AV15">
-        <v>4.2217867287734689</v>
-      </c>
-      <c r="AX15">
+      <c r="BE15">
         <v>4.4332260376972012</v>
       </c>
-      <c r="AZ15">
+      <c r="BG15">
         <v>4.3209471511328488</v>
       </c>
-      <c r="BB15">
+      <c r="BI15">
         <v>4.5205202935934148</v>
       </c>
-      <c r="BH15" t="s">
+      <c r="BK15" t="s">
+        <v>10</v>
+      </c>
+      <c r="BL15" t="s">
         <v>11</v>
       </c>
-      <c r="BI15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D16">
         <v>6.0428004638458797</v>
       </c>
@@ -1494,33 +1593,29 @@
       <c r="AO16" s="1"/>
       <c r="AP16" s="1"/>
       <c r="AQ16" s="1"/>
-      <c r="AV16">
-        <f>AV14-AV15</f>
-        <v>0.43890499145619266</v>
-      </c>
-      <c r="AX16">
-        <f t="shared" ref="AX16" si="4">AX14-AX15</f>
+      <c r="BE16">
+        <f t="shared" ref="BE16" si="4">BE14-BE15</f>
         <v>-4.2934851283323638E-2</v>
       </c>
-      <c r="AZ16">
-        <f t="shared" ref="AZ16" si="5">AZ14-AZ15</f>
+      <c r="BG16">
+        <f t="shared" ref="BG16" si="5">BG14-BG15</f>
         <v>2.5795684075785248</v>
       </c>
-      <c r="BB16">
-        <f t="shared" ref="BB16" si="6">BB14-BB15</f>
+      <c r="BI16">
+        <f t="shared" ref="BI16" si="6">BI14-BI15</f>
         <v>1.2764022491732874</v>
       </c>
-      <c r="BG16" t="s">
-        <v>13</v>
-      </c>
-      <c r="BH16">
+      <c r="BJ16" t="s">
+        <v>12</v>
+      </c>
+      <c r="BK16">
         <v>4.1967017749388837</v>
       </c>
-      <c r="BI16">
+      <c r="BL16">
         <v>4.3209471511328488</v>
       </c>
     </row>
-    <row r="17" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D17">
         <v>5.3331846529911502</v>
       </c>
@@ -1625,35 +1720,43 @@
       <c r="AP17" s="1"/>
       <c r="AQ17" s="1"/>
       <c r="AU17" t="s">
+        <v>18</v>
+      </c>
+      <c r="AX17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AY17" t="s">
+        <v>17</v>
+      </c>
+      <c r="AZ17" t="s">
         <v>20</v>
       </c>
-      <c r="AV17">
-        <f>(AV14/AV15-1)*100</f>
-        <v>10.396190514903282</v>
-      </c>
-      <c r="AX17">
-        <f t="shared" ref="AX17:BB17" si="7">(AX14/AX15-1)*100</f>
+      <c r="BA17" t="s">
+        <v>18</v>
+      </c>
+      <c r="BE17">
+        <f t="shared" ref="BE17:BI17" si="7">(BE14/BE15-1)*100</f>
         <v>-0.96847873124975559</v>
       </c>
-      <c r="AZ17">
+      <c r="BG17">
         <f t="shared" si="7"/>
         <v>59.699142742401378</v>
       </c>
-      <c r="BB17">
+      <c r="BI17">
         <f t="shared" si="7"/>
         <v>28.235737620340593</v>
       </c>
-      <c r="BG17" t="s">
-        <v>14</v>
-      </c>
-      <c r="BH17">
+      <c r="BJ17" t="s">
+        <v>13</v>
+      </c>
+      <c r="BK17">
         <v>6.9237412333723753</v>
       </c>
-      <c r="BI17">
+      <c r="BL17">
         <v>7.2199455498044021</v>
       </c>
     </row>
-    <row r="18" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF18" t="s">
         <v>4</v>
       </c>
@@ -1670,17 +1773,34 @@
       <c r="AU18" t="s">
         <v>4</v>
       </c>
-      <c r="BG18" t="s">
-        <v>15</v>
-      </c>
-      <c r="BH18">
+      <c r="AW18" t="s">
+        <v>21</v>
+      </c>
+      <c r="AX18" s="5">
+        <v>4.7437911226340193</v>
+      </c>
+      <c r="AY18" s="5">
+        <v>4.1967017749388837</v>
+      </c>
+      <c r="AZ18" s="5">
+        <f>AX18-AY18</f>
+        <v>0.54708934769513551</v>
+      </c>
+      <c r="BA18" s="5">
+        <f>(AX18/AY18-1)*100</f>
+        <v>13.036174048919701</v>
+      </c>
+      <c r="BJ18" t="s">
+        <v>14</v>
+      </c>
+      <c r="BK18">
         <v>10.559459629389412</v>
       </c>
-      <c r="BI18">
+      <c r="BL18">
         <v>10.774963435890092</v>
       </c>
     </row>
-    <row r="19" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF19" t="s">
         <v>2</v>
       </c>
@@ -1709,17 +1829,34 @@
       <c r="AV19" t="s">
         <v>6</v>
       </c>
-      <c r="AX19" t="s">
+      <c r="AW19" t="s">
+        <v>22</v>
+      </c>
+      <c r="AX19" s="5">
+        <v>6.9005155587113736</v>
+      </c>
+      <c r="AY19" s="5">
+        <v>4.3209471511328488</v>
+      </c>
+      <c r="AZ19" s="5">
+        <f>AX19-AY19</f>
+        <v>2.5795684075785248</v>
+      </c>
+      <c r="BA19" s="5">
+        <f>(AX19/AY19-1)*100</f>
+        <v>59.699142742401378</v>
+      </c>
+      <c r="BE19" t="s">
         <v>7</v>
       </c>
-      <c r="AZ19" t="s">
+      <c r="BG19" t="s">
         <v>8</v>
       </c>
-      <c r="BB19" t="s">
+      <c r="BI19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D20">
         <v>7.4555122740376101</v>
       </c>
@@ -1836,23 +1973,37 @@
       <c r="AQ20" s="2">
         <v>1.1512915599638371</v>
       </c>
-      <c r="AV20">
-        <v>7.0908315304740643</v>
-      </c>
-      <c r="AX20">
+      <c r="AW20" t="s">
+        <v>23</v>
+      </c>
+      <c r="AX20" s="5">
+        <v>8.0726250323551785</v>
+      </c>
+      <c r="AY20" s="5">
+        <v>6.9237412333723753</v>
+      </c>
+      <c r="AZ20" s="5">
+        <f>AX20-AY20</f>
+        <v>1.1488837989828031</v>
+      </c>
+      <c r="BA20" s="5">
+        <f>(AX20/AY20-1)*100</f>
+        <v>16.593395972760973</v>
+      </c>
+      <c r="BE20">
         <v>8.5893338627309852</v>
       </c>
-      <c r="AZ20">
+      <c r="BG20">
         <v>8.0726250323551785</v>
       </c>
-      <c r="BB20">
+      <c r="BI20">
         <v>9.4339768321203703</v>
       </c>
-      <c r="BH20" t="s">
+      <c r="BK20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D21">
         <v>7.4623693154854198</v>
       </c>
@@ -1957,26 +2108,40 @@
       <c r="AO21" s="2"/>
       <c r="AP21" s="2"/>
       <c r="AQ21" s="2"/>
-      <c r="AV21">
-        <v>6.5052084755275654</v>
-      </c>
-      <c r="AX21">
+      <c r="AW21" t="s">
+        <v>24</v>
+      </c>
+      <c r="AX21" s="5">
+        <v>12.75135957688987</v>
+      </c>
+      <c r="AY21" s="5">
+        <v>7.2199455498044021</v>
+      </c>
+      <c r="AZ21" s="5">
+        <f>AX21-AY21</f>
+        <v>5.5314140270854679</v>
+      </c>
+      <c r="BA21" s="5">
+        <f>(AX21/AY21-1)*100</f>
+        <v>76.612960429255892</v>
+      </c>
+      <c r="BE21">
         <v>9.6382647586513492</v>
       </c>
-      <c r="AZ21">
+      <c r="BG21">
         <v>6.9237412333723753</v>
       </c>
-      <c r="BB21">
+      <c r="BI21">
         <v>10.126514001709587</v>
       </c>
-      <c r="BH21" t="s">
+      <c r="BK21" t="s">
+        <v>10</v>
+      </c>
+      <c r="BL21" t="s">
         <v>11</v>
       </c>
-      <c r="BI21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D22">
         <v>8.2161965336034104</v>
       </c>
@@ -2081,33 +2246,46 @@
       <c r="AO22" s="2"/>
       <c r="AP22" s="2"/>
       <c r="AQ22" s="2"/>
-      <c r="AV22">
-        <f>AV20-AV21</f>
-        <v>0.58562305494649891</v>
-      </c>
-      <c r="AX22">
-        <f t="shared" ref="AX22" si="10">AX20-AX21</f>
+      <c r="AW22" t="s">
+        <v>25</v>
+      </c>
+      <c r="AX22" s="5">
+        <v>12.664070588477017</v>
+      </c>
+      <c r="AY22" s="5">
+        <v>10.559459629389412</v>
+      </c>
+      <c r="AZ22" s="5">
+        <f>AX22-AY22</f>
+        <v>2.104610959087605</v>
+      </c>
+      <c r="BA22" s="5">
+        <f>(AX22/AY22-1)*100</f>
+        <v>19.931047922471222</v>
+      </c>
+      <c r="BE22">
+        <f t="shared" ref="BE22" si="10">BE20-BE21</f>
         <v>-1.048930895920364</v>
       </c>
-      <c r="AZ22">
-        <f t="shared" ref="AZ22" si="11">AZ20-AZ21</f>
+      <c r="BG22">
+        <f t="shared" ref="BG22" si="11">BG20-BG21</f>
         <v>1.1488837989828031</v>
       </c>
-      <c r="BB22">
-        <f t="shared" ref="BB22" si="12">BB20-BB21</f>
+      <c r="BI22">
+        <f t="shared" ref="BI22" si="12">BI20-BI21</f>
         <v>-0.69253716958921707</v>
       </c>
-      <c r="BG22" t="s">
-        <v>13</v>
-      </c>
-      <c r="BH22">
+      <c r="BJ22" t="s">
+        <v>12</v>
+      </c>
+      <c r="BK22">
         <v>4.1030539582227208</v>
       </c>
-      <c r="BI22">
+      <c r="BL22">
         <v>4.2217867287734689</v>
       </c>
     </row>
-    <row r="23" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D23">
         <v>9.7609187895834406</v>
       </c>
@@ -2213,35 +2391,48 @@
       <c r="AP23" s="2"/>
       <c r="AQ23" s="2"/>
       <c r="AU23" t="s">
-        <v>20</v>
-      </c>
-      <c r="AV23">
-        <f>(AV20/AV21-1)*100</f>
-        <v>9.002371824816958</v>
-      </c>
-      <c r="AX23">
-        <f t="shared" ref="AX23:BB23" si="13">(AX20/AX21-1)*100</f>
+        <v>18</v>
+      </c>
+      <c r="AW23" t="s">
+        <v>26</v>
+      </c>
+      <c r="AX23" s="5">
+        <v>23.38056567610445</v>
+      </c>
+      <c r="AY23" s="5">
+        <v>10.774963435890092</v>
+      </c>
+      <c r="AZ23" s="5">
+        <f>AX23-AY23</f>
+        <v>12.605602240214358</v>
+      </c>
+      <c r="BA23" s="5">
+        <f>(AX23/AY23-1)*100</f>
+        <v>116.98974493246661</v>
+      </c>
+      <c r="BE23">
+        <f t="shared" ref="BE23:BI23" si="13">(BE20/BE21-1)*100</f>
         <v>-10.882984875247793</v>
       </c>
-      <c r="AZ23">
+      <c r="BG23">
         <f t="shared" si="13"/>
         <v>16.593395972760973</v>
       </c>
-      <c r="BB23">
+      <c r="BI23">
         <f t="shared" si="13"/>
         <v>-6.8388506594895482</v>
       </c>
-      <c r="BG23" t="s">
-        <v>14</v>
-      </c>
-      <c r="BH23">
+      <c r="BJ23" t="s">
+        <v>13</v>
+      </c>
+      <c r="BK23">
         <v>6.5052084755275654</v>
       </c>
-      <c r="BI23">
+      <c r="BL23">
         <v>6.6160894971757473</v>
       </c>
     </row>
-    <row r="24" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF24" t="s">
         <v>4</v>
       </c>
@@ -2259,17 +2450,17 @@
       <c r="AU24" t="s">
         <v>4</v>
       </c>
-      <c r="BG24" t="s">
-        <v>15</v>
-      </c>
-      <c r="BH24">
+      <c r="BJ24" t="s">
+        <v>14</v>
+      </c>
+      <c r="BK24">
         <v>8.5196521018960976</v>
       </c>
-      <c r="BI24">
+      <c r="BL24">
         <v>8.4025380938040506</v>
       </c>
     </row>
-    <row r="25" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF25" t="s">
         <v>3</v>
       </c>
@@ -2298,17 +2489,17 @@
       <c r="AV25" t="s">
         <v>6</v>
       </c>
-      <c r="AX25" t="s">
+      <c r="BE25" t="s">
         <v>7</v>
       </c>
-      <c r="AZ25" t="s">
+      <c r="BG25" t="s">
         <v>8</v>
       </c>
-      <c r="BB25" t="s">
+      <c r="BI25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D26">
         <v>7.85702009299</v>
       </c>
@@ -2425,20 +2616,17 @@
       <c r="AQ26" s="2">
         <v>3.0652320075246342</v>
       </c>
-      <c r="AV26">
-        <v>8.0174685918405455</v>
-      </c>
-      <c r="AX26">
+      <c r="BE26">
         <v>8.6190510001893657</v>
       </c>
-      <c r="AZ26">
+      <c r="BG26">
         <v>12.75135957688987</v>
       </c>
-      <c r="BB26">
+      <c r="BI26">
         <v>10.902809543502425</v>
       </c>
     </row>
-    <row r="27" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D27">
         <v>6.2422008801175304</v>
       </c>
@@ -2543,20 +2731,29 @@
       <c r="AO27" s="2"/>
       <c r="AP27" s="2"/>
       <c r="AQ27" s="2"/>
-      <c r="AV27">
-        <v>6.6160894971757473</v>
-      </c>
-      <c r="AX27">
+      <c r="AX27" t="s">
+        <v>19</v>
+      </c>
+      <c r="AY27" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ27" t="s">
+        <v>20</v>
+      </c>
+      <c r="BA27" t="s">
+        <v>18</v>
+      </c>
+      <c r="BE27">
         <v>9.8018396754248034</v>
       </c>
-      <c r="AZ27">
+      <c r="BG27">
         <v>7.2199455498044021</v>
       </c>
-      <c r="BB27">
+      <c r="BI27">
         <v>10.063961470180555</v>
       </c>
     </row>
-    <row r="28" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D28">
         <v>12.0287094898323</v>
       </c>
@@ -2661,24 +2858,37 @@
       <c r="AO28" s="2"/>
       <c r="AP28" s="2"/>
       <c r="AQ28" s="2"/>
-      <c r="AV28">
-        <f>AV26-AV27</f>
-        <v>1.4013790946647982</v>
-      </c>
-      <c r="AX28">
-        <f t="shared" ref="AX28" si="14">AX26-AX27</f>
+      <c r="AW28" t="s">
+        <v>21</v>
+      </c>
+      <c r="AX28" s="5">
+        <v>4.3145492000507879</v>
+      </c>
+      <c r="AY28" s="5">
+        <v>4.4580286638103868</v>
+      </c>
+      <c r="AZ28" s="5">
+        <f>AX28-AY28</f>
+        <v>-0.14347946375959886</v>
+      </c>
+      <c r="BA28" s="5">
+        <f>(AX28/AY28-1)*100</f>
+        <v>-3.2184509023987173</v>
+      </c>
+      <c r="BE28">
+        <f t="shared" ref="BE28" si="14">BE26-BE27</f>
         <v>-1.1827886752354377</v>
       </c>
-      <c r="AZ28">
-        <f t="shared" ref="AZ28" si="15">AZ26-AZ27</f>
+      <c r="BG28">
+        <f t="shared" ref="BG28" si="15">BG26-BG27</f>
         <v>5.5314140270854679</v>
       </c>
-      <c r="BB28">
-        <f t="shared" ref="BB28" si="16">BB26-BB27</f>
+      <c r="BI28">
+        <f t="shared" ref="BI28" si="16">BI26-BI27</f>
         <v>0.83884807332186995</v>
       </c>
     </row>
-    <row r="29" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D29">
         <v>12.2233497883651</v>
       </c>
@@ -2784,26 +2994,39 @@
       <c r="AP29" s="2"/>
       <c r="AQ29" s="2"/>
       <c r="AU29" t="s">
-        <v>20</v>
-      </c>
-      <c r="AV29">
-        <f>(AV26/AV27-1)*100</f>
-        <v>21.181380561176113</v>
-      </c>
-      <c r="AX29">
-        <f t="shared" ref="AX29:BB29" si="17">(AX26/AX27-1)*100</f>
+        <v>18</v>
+      </c>
+      <c r="AW29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AX29" s="5">
+        <v>4.3902911864138776</v>
+      </c>
+      <c r="AY29" s="5">
+        <v>4.4332260376972012</v>
+      </c>
+      <c r="AZ29" s="5">
+        <f>AX29-AY29</f>
+        <v>-4.2934851283323638E-2</v>
+      </c>
+      <c r="BA29" s="5">
+        <f>(AX29/AY29-1)*100</f>
+        <v>-0.96847873124975559</v>
+      </c>
+      <c r="BE29">
+        <f t="shared" ref="BE29:BI29" si="17">(BE26/BE27-1)*100</f>
         <v>-12.067006953816318</v>
       </c>
-      <c r="AZ29">
+      <c r="BG29">
         <f t="shared" si="17"/>
         <v>76.612960429255892</v>
       </c>
-      <c r="BB29">
+      <c r="BI29">
         <f t="shared" si="17"/>
         <v>8.3351677747114827</v>
       </c>
     </row>
-    <row r="30" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF30" t="s">
         <v>5</v>
       </c>
@@ -2821,8 +3044,25 @@
       <c r="AU30" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AW30" t="s">
+        <v>23</v>
+      </c>
+      <c r="AX30" s="5">
+        <v>8.5893338627309852</v>
+      </c>
+      <c r="AY30" s="5">
+        <v>9.6382647586513492</v>
+      </c>
+      <c r="AZ30" s="5">
+        <f>AX30-AY30</f>
+        <v>-1.048930895920364</v>
+      </c>
+      <c r="BA30" s="5">
+        <f>(AX30/AY30-1)*100</f>
+        <v>-10.882984875247793</v>
+      </c>
+    </row>
+    <row r="31" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF31" t="s">
         <v>2</v>
       </c>
@@ -2851,17 +3091,34 @@
       <c r="AV31" t="s">
         <v>6</v>
       </c>
-      <c r="AX31" t="s">
+      <c r="AW31" t="s">
+        <v>24</v>
+      </c>
+      <c r="AX31" s="5">
+        <v>8.6190510001893657</v>
+      </c>
+      <c r="AY31" s="5">
+        <v>9.8018396754248034</v>
+      </c>
+      <c r="AZ31" s="5">
+        <f>AX31-AY31</f>
+        <v>-1.1827886752354377</v>
+      </c>
+      <c r="BA31" s="5">
+        <f>(AX31/AY31-1)*100</f>
+        <v>-12.067006953816318</v>
+      </c>
+      <c r="BE31" t="s">
         <v>7</v>
       </c>
-      <c r="AZ31" t="s">
+      <c r="BG31" t="s">
         <v>8</v>
       </c>
-      <c r="BB31" t="s">
+      <c r="BI31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:64" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D32">
         <v>9.14871860127659</v>
       </c>
@@ -2978,20 +3235,34 @@
       <c r="AQ32" s="2">
         <v>2.7167443958416784</v>
       </c>
-      <c r="AV32">
-        <v>9.3416814204142913</v>
-      </c>
-      <c r="AX32">
+      <c r="AW32" t="s">
+        <v>25</v>
+      </c>
+      <c r="AX32" s="5">
         <v>15.374403149212615</v>
       </c>
-      <c r="AZ32">
+      <c r="AY32" s="5">
+        <v>16.216907711420916</v>
+      </c>
+      <c r="AZ32" s="5">
+        <f>AX32-AY32</f>
+        <v>-0.84250456220830117</v>
+      </c>
+      <c r="BA32" s="5">
+        <f>(AX32/AY32-1)*100</f>
+        <v>-5.1952232645127499</v>
+      </c>
+      <c r="BE32">
+        <v>15.374403149212615</v>
+      </c>
+      <c r="BG32">
         <v>12.664070588477017</v>
       </c>
-      <c r="BB32">
+      <c r="BI32">
         <v>18.711215843700355</v>
       </c>
     </row>
-    <row r="33" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D33">
         <v>16.541181728659499</v>
       </c>
@@ -3096,20 +3367,34 @@
       <c r="AO33" s="2"/>
       <c r="AP33" s="2"/>
       <c r="AQ33" s="2"/>
-      <c r="AV33">
-        <v>8.5196521018960976</v>
-      </c>
-      <c r="AX33">
+      <c r="AW33" t="s">
+        <v>26</v>
+      </c>
+      <c r="AX33" s="5">
+        <v>16.987513012340507</v>
+      </c>
+      <c r="AY33" s="5">
+        <v>15.944082701894363</v>
+      </c>
+      <c r="AZ33" s="5">
+        <f>AX33-AY33</f>
+        <v>1.0434303104461442</v>
+      </c>
+      <c r="BA33" s="5">
+        <f>(AX33/AY33-1)*100</f>
+        <v>6.5443107010613399</v>
+      </c>
+      <c r="BE33">
         <v>16.216907711420916</v>
       </c>
-      <c r="AZ33">
+      <c r="BG33">
         <v>10.559459629389412</v>
       </c>
-      <c r="BB33">
+      <c r="BI33">
         <v>19.104781491799571</v>
       </c>
     </row>
-    <row r="34" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D34">
         <v>10.9660527770196</v>
       </c>
@@ -3214,24 +3499,20 @@
       <c r="AO34" s="2"/>
       <c r="AP34" s="2"/>
       <c r="AQ34" s="2"/>
-      <c r="AV34">
-        <f>AV32-AV33</f>
-        <v>0.82202931851819372</v>
-      </c>
-      <c r="AX34">
-        <f t="shared" ref="AX34" si="18">AX32-AX33</f>
+      <c r="BE34">
+        <f t="shared" ref="BE34" si="18">BE32-BE33</f>
         <v>-0.84250456220830117</v>
       </c>
-      <c r="AZ34">
-        <f t="shared" ref="AZ34" si="19">AZ32-AZ33</f>
+      <c r="BG34">
+        <f t="shared" ref="BG34" si="19">BG32-BG33</f>
         <v>2.104610959087605</v>
       </c>
-      <c r="BB34">
-        <f t="shared" ref="BB34" si="20">BB32-BB33</f>
+      <c r="BI34">
+        <f t="shared" ref="BI34" si="20">BI32-BI33</f>
         <v>-0.39356564809921579</v>
       </c>
     </row>
-    <row r="35" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D35">
         <v>19.640271484319602</v>
       </c>
@@ -3337,26 +3618,22 @@
       <c r="AP35" s="2"/>
       <c r="AQ35" s="2"/>
       <c r="AU35" t="s">
-        <v>20</v>
-      </c>
-      <c r="AV35">
-        <f>(AV32/AV33-1)*100</f>
-        <v>9.6486254213977496</v>
-      </c>
-      <c r="AX35">
-        <f t="shared" ref="AX35:BB35" si="21">(AX32/AX33-1)*100</f>
+        <v>18</v>
+      </c>
+      <c r="BE35">
+        <f t="shared" ref="BE35:BI35" si="21">(BE32/BE33-1)*100</f>
         <v>-5.1952232645127499</v>
       </c>
-      <c r="AZ35">
+      <c r="BG35">
         <f t="shared" si="21"/>
         <v>19.931047922471222</v>
       </c>
-      <c r="BB35">
+      <c r="BI35">
         <f t="shared" si="21"/>
         <v>-2.0600374218786466</v>
       </c>
     </row>
-    <row r="36" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF36" t="s">
         <v>5</v>
       </c>
@@ -3374,8 +3651,20 @@
       <c r="AU36" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AX36" t="s">
+        <v>19</v>
+      </c>
+      <c r="AY36" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ36" t="s">
+        <v>20</v>
+      </c>
+      <c r="BA36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AF37" t="s">
         <v>3</v>
       </c>
@@ -3404,17 +3693,34 @@
       <c r="AV37" t="s">
         <v>6</v>
       </c>
-      <c r="AX37" t="s">
+      <c r="AW37" t="s">
+        <v>21</v>
+      </c>
+      <c r="AX37" s="5">
+        <v>4.2568917664147978</v>
+      </c>
+      <c r="AY37" s="5">
+        <v>4.5340149921451269</v>
+      </c>
+      <c r="AZ37" s="5">
+        <f>AX37-AY37</f>
+        <v>-0.2771232257303291</v>
+      </c>
+      <c r="BA37" s="5">
+        <f>(AX37/AY37-1)*100</f>
+        <v>-6.1120932817916636</v>
+      </c>
+      <c r="BE37" t="s">
         <v>7</v>
       </c>
-      <c r="AZ37" t="s">
+      <c r="BG37" t="s">
         <v>8</v>
       </c>
-      <c r="BB37" t="s">
+      <c r="BI37" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D38">
         <v>12.186678730118</v>
       </c>
@@ -3531,20 +3837,34 @@
       <c r="AQ38" s="2">
         <v>11.021409584412559</v>
       </c>
-      <c r="AV38">
-        <v>12.186117717401205</v>
-      </c>
-      <c r="AX38">
+      <c r="AW38" t="s">
+        <v>22</v>
+      </c>
+      <c r="AX38" s="5">
+        <v>5.7969225427667022</v>
+      </c>
+      <c r="AY38" s="5">
+        <v>4.5205202935934148</v>
+      </c>
+      <c r="AZ38" s="5">
+        <f>AX38-AY38</f>
+        <v>1.2764022491732874</v>
+      </c>
+      <c r="BA38" s="5">
+        <f>(AX38/AY38-1)*100</f>
+        <v>28.235737620340593</v>
+      </c>
+      <c r="BE38">
         <v>16.987513012340507</v>
       </c>
-      <c r="AZ38">
+      <c r="BG38">
         <v>23.38056567610445</v>
       </c>
-      <c r="BB38">
+      <c r="BI38">
         <v>29.32912838340696</v>
       </c>
     </row>
-    <row r="39" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D39">
         <v>20.4091701925243</v>
       </c>
@@ -3648,20 +3968,34 @@
       <c r="AO39" s="1"/>
       <c r="AP39" s="1"/>
       <c r="AQ39" s="1"/>
-      <c r="AV39">
-        <v>8.4025380938040506</v>
-      </c>
-      <c r="AX39">
+      <c r="AW39" t="s">
+        <v>23</v>
+      </c>
+      <c r="AX39" s="5">
+        <v>9.4339768321203703</v>
+      </c>
+      <c r="AY39" s="5">
+        <v>10.126514001709587</v>
+      </c>
+      <c r="AZ39" s="5">
+        <f>AX39-AY39</f>
+        <v>-0.69253716958921707</v>
+      </c>
+      <c r="BA39" s="5">
+        <f>(AX39/AY39-1)*100</f>
+        <v>-6.8388506594895482</v>
+      </c>
+      <c r="BE39">
         <v>15.944082701894363</v>
       </c>
-      <c r="AZ39">
+      <c r="BG39">
         <v>10.774963435890092</v>
       </c>
-      <c r="BB39">
+      <c r="BI39">
         <v>18.904530166296727</v>
       </c>
     </row>
-    <row r="40" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D40">
         <v>29.3160265856596</v>
       </c>
@@ -3765,24 +4099,37 @@
       <c r="AO40" s="1"/>
       <c r="AP40" s="1"/>
       <c r="AQ40" s="1"/>
-      <c r="AV40">
-        <f>AV38-AV39</f>
-        <v>3.7835796235971539</v>
-      </c>
-      <c r="AX40">
-        <f t="shared" ref="AX40" si="24">AX38-AX39</f>
+      <c r="AW40" t="s">
+        <v>24</v>
+      </c>
+      <c r="AX40" s="5">
+        <v>10.902809543502425</v>
+      </c>
+      <c r="AY40" s="5">
+        <v>10.063961470180555</v>
+      </c>
+      <c r="AZ40" s="5">
+        <f>AX40-AY40</f>
+        <v>0.83884807332186995</v>
+      </c>
+      <c r="BA40" s="5">
+        <f>(AX40/AY40-1)*100</f>
+        <v>8.3351677747114827</v>
+      </c>
+      <c r="BE40">
+        <f t="shared" ref="BE40" si="24">BE38-BE39</f>
         <v>1.0434303104461442</v>
       </c>
-      <c r="AZ40">
-        <f t="shared" ref="AZ40" si="25">AZ38-AZ39</f>
+      <c r="BG40">
+        <f t="shared" ref="BG40" si="25">BG38-BG39</f>
         <v>12.605602240214358</v>
       </c>
-      <c r="BB40">
-        <f t="shared" ref="BB40" si="26">BB38-BB39</f>
+      <c r="BI40">
+        <f t="shared" ref="BI40" si="26">BI38-BI39</f>
         <v>10.424598217110233</v>
       </c>
     </row>
-    <row r="41" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D41">
         <v>21.7314376586049</v>
       </c>
@@ -3887,26 +4234,39 @@
       <c r="AP41" s="1"/>
       <c r="AQ41" s="1"/>
       <c r="AU41" t="s">
-        <v>20</v>
-      </c>
-      <c r="AV41">
-        <f>(AV38/AV39-1)*100</f>
-        <v>45.029008870392715</v>
-      </c>
-      <c r="AX41">
-        <f t="shared" ref="AX41:BB41" si="27">(AX38/AX39-1)*100</f>
+        <v>18</v>
+      </c>
+      <c r="AW41" t="s">
+        <v>25</v>
+      </c>
+      <c r="AX41" s="5">
+        <v>18.711215843700355</v>
+      </c>
+      <c r="AY41" s="5">
+        <v>19.104781491799571</v>
+      </c>
+      <c r="AZ41" s="5">
+        <f>AX41-AY41</f>
+        <v>-0.39356564809921579</v>
+      </c>
+      <c r="BA41" s="5">
+        <f>(AX41/AY41-1)*100</f>
+        <v>-2.0600374218786466</v>
+      </c>
+      <c r="BE41">
+        <f t="shared" ref="BE41:BI41" si="27">(BE38/BE39-1)*100</f>
         <v>6.5443107010613399</v>
       </c>
-      <c r="AZ41">
+      <c r="BG41">
         <f t="shared" si="27"/>
         <v>116.98974493246661</v>
       </c>
-      <c r="BB41">
+      <c r="BI41">
         <f t="shared" si="27"/>
         <v>55.143386931114314</v>
       </c>
     </row>
-    <row r="42" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AJ42" s="2"/>
       <c r="AK42" s="2"/>
       <c r="AM42" s="2"/>
@@ -3914,8 +4274,25 @@
       <c r="AO42" s="1"/>
       <c r="AP42" s="1"/>
       <c r="AQ42" s="1"/>
-    </row>
-    <row r="43" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AW42" t="s">
+        <v>26</v>
+      </c>
+      <c r="AX42" s="5">
+        <v>29.32912838340696</v>
+      </c>
+      <c r="AY42" s="5">
+        <v>18.904530166296727</v>
+      </c>
+      <c r="AZ42" s="5">
+        <f>AX42-AY42</f>
+        <v>10.424598217110233</v>
+      </c>
+      <c r="BA42" s="5">
+        <f>(AX42/AY42-1)*100</f>
+        <v>55.143386931114314</v>
+      </c>
+    </row>
+    <row r="43" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AJ43" s="2"/>
       <c r="AK43" s="2"/>
       <c r="AM43" s="1"/>
@@ -3924,7 +4301,7 @@
       <c r="AP43" s="1"/>
       <c r="AQ43" s="1"/>
     </row>
-    <row r="44" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AJ44" s="2"/>
       <c r="AK44" s="2"/>
       <c r="AM44" s="1"/>
@@ -3933,7 +4310,7 @@
       <c r="AP44" s="1"/>
       <c r="AQ44" s="1"/>
     </row>
-    <row r="45" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AJ45" s="2"/>
       <c r="AK45" s="2"/>
       <c r="AM45" s="2"/>
@@ -3942,7 +4319,7 @@
       <c r="AP45" s="1"/>
       <c r="AQ45" s="1"/>
     </row>
-    <row r="46" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AJ46" s="2"/>
       <c r="AK46" s="2"/>
       <c r="AM46" s="2"/>
@@ -3951,7 +4328,7 @@
       <c r="AP46" s="1"/>
       <c r="AQ46" s="1"/>
     </row>
-    <row r="47" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AJ47" s="2"/>
       <c r="AK47" s="2"/>
       <c r="AM47" s="2"/>
@@ -3960,7 +4337,7 @@
       <c r="AP47" s="1"/>
       <c r="AQ47" s="1"/>
     </row>
-    <row r="48" spans="4:54" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:61" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AJ48" s="2"/>
       <c r="AK48" s="2"/>
       <c r="AM48" s="2"/>
@@ -4356,4 +4733,2814 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D6:AS41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AK10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AS23" sqref="AS23:AS25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="6" spans="4:45" x14ac:dyDescent="0.25">
+      <c r="AF6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AF7" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK7" s="2"/>
+    </row>
+    <row r="8" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>0.88362012059404504</v>
+      </c>
+      <c r="E8">
+        <v>1.6792899067996201</v>
+      </c>
+      <c r="F8">
+        <v>2.1442552191781301</v>
+      </c>
+      <c r="G8">
+        <v>1.1672217151334401</v>
+      </c>
+      <c r="H8">
+        <v>1.8393026970303401</v>
+      </c>
+      <c r="I8">
+        <v>1.77038765125288</v>
+      </c>
+      <c r="J8">
+        <v>1.9294979171878499</v>
+      </c>
+      <c r="K8">
+        <v>1.7013150971336199</v>
+      </c>
+      <c r="L8">
+        <v>1.8803406842763799</v>
+      </c>
+      <c r="M8">
+        <v>1.91369033596241</v>
+      </c>
+      <c r="N8">
+        <v>1.6864178147170401</v>
+      </c>
+      <c r="O8">
+        <v>1.95864246274229</v>
+      </c>
+      <c r="P8">
+        <v>1.8966271874546601</v>
+      </c>
+      <c r="Q8">
+        <v>1.79208666056044</v>
+      </c>
+      <c r="R8">
+        <v>1.0615853837276099</v>
+      </c>
+      <c r="S8">
+        <v>1.9459862044542999</v>
+      </c>
+      <c r="T8">
+        <v>1.0391623708128199</v>
+      </c>
+      <c r="U8">
+        <v>0.90007512736929596</v>
+      </c>
+      <c r="V8">
+        <v>1.9361445010182801</v>
+      </c>
+      <c r="W8">
+        <v>1.8771424408084401</v>
+      </c>
+      <c r="X8">
+        <v>1.8083139778647199</v>
+      </c>
+      <c r="Y8">
+        <v>1.71601629810087</v>
+      </c>
+      <c r="Z8">
+        <v>1.7987825396308099</v>
+      </c>
+      <c r="AA8">
+        <v>0.99113041037257998</v>
+      </c>
+      <c r="AB8">
+        <v>1.9856264639477901</v>
+      </c>
+      <c r="AC8">
+        <v>1.8900172693019399</v>
+      </c>
+      <c r="AD8">
+        <v>1.1694532486607201</v>
+      </c>
+      <c r="AE8">
+        <v>1.8157043588635</v>
+      </c>
+      <c r="AF8">
+        <v>1.07200565869885</v>
+      </c>
+      <c r="AG8">
+        <v>1.20214950605454</v>
+      </c>
+      <c r="AJ8" s="2">
+        <f>AVERAGE(D8:AG8)</f>
+        <v>1.6150663743236735</v>
+      </c>
+      <c r="AK8" s="2">
+        <f>_xlfn.STDEV.S(D8:AG8)</f>
+        <v>0.39004825557847944</v>
+      </c>
+      <c r="AL8">
+        <v>1.6150663743236735</v>
+      </c>
+      <c r="AP8">
+        <v>1.6150663743236735</v>
+      </c>
+      <c r="AQ8">
+        <v>2.1562636783693474</v>
+      </c>
+      <c r="AR8">
+        <v>1.6690253864999696</v>
+      </c>
+      <c r="AS8">
+        <v>2.0841411531572165</v>
+      </c>
+    </row>
+    <row r="9" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>1.8326960685442699</v>
+      </c>
+      <c r="E9">
+        <v>2.2885067949881401</v>
+      </c>
+      <c r="F9">
+        <v>2.3776932565434801</v>
+      </c>
+      <c r="G9">
+        <v>2.3155352811096401</v>
+      </c>
+      <c r="H9">
+        <v>2.1509294229239702</v>
+      </c>
+      <c r="I9">
+        <v>1.9300912246150499</v>
+      </c>
+      <c r="J9">
+        <v>1.8373727789852099</v>
+      </c>
+      <c r="K9">
+        <v>2.1191816173551001</v>
+      </c>
+      <c r="L9">
+        <v>1.65865443332351</v>
+      </c>
+      <c r="M9">
+        <v>2.7561551338605801</v>
+      </c>
+      <c r="N9">
+        <v>2.2450055117594401</v>
+      </c>
+      <c r="O9">
+        <v>1.97933391720277</v>
+      </c>
+      <c r="P9">
+        <v>2.41026546658148</v>
+      </c>
+      <c r="Q9">
+        <v>1.5113067120864001</v>
+      </c>
+      <c r="R9">
+        <v>1.85098012920453</v>
+      </c>
+      <c r="S9">
+        <v>1.9055218579998801</v>
+      </c>
+      <c r="T9">
+        <v>2.57182829945046</v>
+      </c>
+      <c r="U9">
+        <v>1.1663088485477799</v>
+      </c>
+      <c r="V9">
+        <v>2.4604051172694898</v>
+      </c>
+      <c r="W9">
+        <v>2.5767435457534802</v>
+      </c>
+      <c r="X9">
+        <v>2.4862864715092798</v>
+      </c>
+      <c r="Y9">
+        <v>1.8813521734421099</v>
+      </c>
+      <c r="Z9">
+        <v>0.88233725766512805</v>
+      </c>
+      <c r="AA9">
+        <v>1.89179846776299</v>
+      </c>
+      <c r="AB9">
+        <v>2.1683335080165298</v>
+      </c>
+      <c r="AC9">
+        <v>2.84397231310265</v>
+      </c>
+      <c r="AD9">
+        <v>2.6232733871290699</v>
+      </c>
+      <c r="AE9">
+        <v>2.6023018874934198</v>
+      </c>
+      <c r="AF9">
+        <v>2.00419548604608</v>
+      </c>
+      <c r="AG9">
+        <v>3.3595439808085099</v>
+      </c>
+      <c r="AJ9" s="2">
+        <f>AVERAGE(D9:AG9)</f>
+        <v>2.1562636783693474</v>
+      </c>
+      <c r="AK9" s="2">
+        <f>_xlfn.STDEV.S(D9:AG9)</f>
+        <v>0.50153311029415026</v>
+      </c>
+      <c r="AL9">
+        <v>2.1562636783693474</v>
+      </c>
+      <c r="AP9">
+        <v>1.7179855106648354</v>
+      </c>
+      <c r="AQ9">
+        <v>2.205061202046287</v>
+      </c>
+      <c r="AR9">
+        <v>1.9837340336719673</v>
+      </c>
+      <c r="AS9">
+        <v>2.2847399602446976</v>
+      </c>
+    </row>
+    <row r="10" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>2.2635051903355299</v>
+      </c>
+      <c r="E10">
+        <v>2.09745421123099</v>
+      </c>
+      <c r="F10">
+        <v>1.36619521284879</v>
+      </c>
+      <c r="G10">
+        <v>1.8516320458312101</v>
+      </c>
+      <c r="H10">
+        <v>1.9106211447120101</v>
+      </c>
+      <c r="I10">
+        <v>1.8460610505638499</v>
+      </c>
+      <c r="J10">
+        <v>1.8128275158410101</v>
+      </c>
+      <c r="K10">
+        <v>1.7965566468919401</v>
+      </c>
+      <c r="L10">
+        <v>1.80871176558862</v>
+      </c>
+      <c r="M10">
+        <v>2.1465313081841599</v>
+      </c>
+      <c r="N10">
+        <v>2.1187321881101302</v>
+      </c>
+      <c r="O10">
+        <v>1.0704293130536999</v>
+      </c>
+      <c r="P10">
+        <v>2.2203806977890999</v>
+      </c>
+      <c r="Q10">
+        <v>1.3313424340857201</v>
+      </c>
+      <c r="R10">
+        <v>1.1144356240914</v>
+      </c>
+      <c r="S10">
+        <v>1.2342392109346101</v>
+      </c>
+      <c r="T10">
+        <v>1.0002872744726301</v>
+      </c>
+      <c r="U10">
+        <v>1.1100500432429801</v>
+      </c>
+      <c r="V10">
+        <v>1.8415014417345501</v>
+      </c>
+      <c r="W10">
+        <v>1.84937976546192</v>
+      </c>
+      <c r="X10">
+        <v>2.1215009348597902</v>
+      </c>
+      <c r="Y10">
+        <v>1.0183383661157099</v>
+      </c>
+      <c r="Z10">
+        <v>1.91816832384479</v>
+      </c>
+      <c r="AA10">
+        <v>1.1584920526567699</v>
+      </c>
+      <c r="AB10">
+        <v>2.1101037725928098</v>
+      </c>
+      <c r="AC10">
+        <v>2.1141318796720401</v>
+      </c>
+      <c r="AD10">
+        <v>1.07128707497371</v>
+      </c>
+      <c r="AE10">
+        <v>1.17575895295762</v>
+      </c>
+      <c r="AF10">
+        <v>1.16161820719433</v>
+      </c>
+      <c r="AG10">
+        <v>2.4304879451266799</v>
+      </c>
+      <c r="AJ10" s="2">
+        <f t="shared" ref="AJ10:AL17" si="0">AVERAGE(D10:AG10)</f>
+        <v>1.6690253864999696</v>
+      </c>
+      <c r="AK10" s="2">
+        <f t="shared" ref="AK10:AK17" si="1">_xlfn.STDEV.S(D10:AG10)</f>
+        <v>0.45918650763162494</v>
+      </c>
+      <c r="AL10">
+        <v>1.6690253864999696</v>
+      </c>
+      <c r="AP10">
+        <v>3.4727194131047758</v>
+      </c>
+      <c r="AQ10">
+        <v>4.6203290330256275</v>
+      </c>
+      <c r="AR10">
+        <v>3.8604717711463024</v>
+      </c>
+      <c r="AS10">
+        <v>4.7214033657582339</v>
+      </c>
+    </row>
+    <row r="11" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>1.5374449569973101</v>
+      </c>
+      <c r="E11">
+        <v>2.0637148825349301</v>
+      </c>
+      <c r="F11">
+        <v>2.8153901375869199</v>
+      </c>
+      <c r="G11">
+        <v>1.8235929354649301</v>
+      </c>
+      <c r="H11">
+        <v>1.7416408045295499</v>
+      </c>
+      <c r="I11">
+        <v>2.9771820100833901</v>
+      </c>
+      <c r="J11">
+        <v>1.8110529054800899</v>
+      </c>
+      <c r="K11">
+        <v>2.4517703542695601</v>
+      </c>
+      <c r="L11">
+        <v>1.1867881748095599</v>
+      </c>
+      <c r="M11">
+        <v>2.0191848888774002</v>
+      </c>
+      <c r="N11">
+        <v>1.14928676603375</v>
+      </c>
+      <c r="O11">
+        <v>1.85948112839514</v>
+      </c>
+      <c r="P11">
+        <v>1.94097624645889</v>
+      </c>
+      <c r="Q11">
+        <v>1.12536596168589</v>
+      </c>
+      <c r="R11">
+        <v>1.7826792538732199</v>
+      </c>
+      <c r="S11">
+        <v>2.2288686348486002</v>
+      </c>
+      <c r="T11">
+        <v>1.9048326292784701</v>
+      </c>
+      <c r="U11">
+        <v>2.4435111890934298</v>
+      </c>
+      <c r="V11">
+        <v>3.0538008473137301</v>
+      </c>
+      <c r="W11">
+        <v>1.02638922987796</v>
+      </c>
+      <c r="X11">
+        <v>2.8373428560037501</v>
+      </c>
+      <c r="Y11">
+        <v>2.0231835077889899</v>
+      </c>
+      <c r="Z11">
+        <v>1.85427531788311</v>
+      </c>
+      <c r="AA11">
+        <v>3.8309908343371202</v>
+      </c>
+      <c r="AB11">
+        <v>2.8463394028389501</v>
+      </c>
+      <c r="AC11">
+        <v>1.86351209350334</v>
+      </c>
+      <c r="AD11">
+        <v>1.93757372475861</v>
+      </c>
+      <c r="AE11">
+        <v>2.4919902584109499</v>
+      </c>
+      <c r="AF11">
+        <v>1.5796243298087</v>
+      </c>
+      <c r="AG11">
+        <v>2.31644833189026</v>
+      </c>
+      <c r="AJ11" s="2">
+        <f t="shared" si="0"/>
+        <v>2.0841411531572165</v>
+      </c>
+      <c r="AK11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.6387918956434866</v>
+      </c>
+      <c r="AL11">
+        <v>2.0841411531572165</v>
+      </c>
+      <c r="AP11">
+        <v>3.8197596205068676</v>
+      </c>
+      <c r="AQ11">
+        <v>4.6782716422325175</v>
+      </c>
+      <c r="AR11">
+        <v>5.5650747070751079</v>
+      </c>
+      <c r="AS11">
+        <v>5.4250457018306415</v>
+      </c>
+    </row>
+    <row r="12" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AI12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ12" s="2"/>
+      <c r="AK12" s="2"/>
+      <c r="AP12">
+        <v>4.825152644366649</v>
+      </c>
+      <c r="AQ12">
+        <v>8.1297108955336537</v>
+      </c>
+      <c r="AR12">
+        <v>5.7203499395237367</v>
+      </c>
+      <c r="AS12">
+        <v>8.7698047774647314</v>
+      </c>
+    </row>
+    <row r="13" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AF13" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK13" s="2"/>
+      <c r="AP13">
+        <v>6.1724764986002869</v>
+      </c>
+      <c r="AQ13">
+        <v>9.4669736430625715</v>
+      </c>
+      <c r="AR13">
+        <v>9.6695592331222908</v>
+      </c>
+      <c r="AS13">
+        <v>11.457843891273024</v>
+      </c>
+    </row>
+    <row r="14" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>1.2777833521635</v>
+      </c>
+      <c r="E14">
+        <v>1.79432367537925</v>
+      </c>
+      <c r="F14">
+        <v>2.1183325988132098</v>
+      </c>
+      <c r="G14">
+        <v>1.8461256384407401</v>
+      </c>
+      <c r="H14">
+        <v>2.2418080101529401</v>
+      </c>
+      <c r="I14">
+        <v>2.4520612274665901</v>
+      </c>
+      <c r="J14">
+        <v>2.2359590103724898</v>
+      </c>
+      <c r="K14">
+        <v>1.1893368859586999</v>
+      </c>
+      <c r="L14">
+        <v>1.7488379696523999</v>
+      </c>
+      <c r="M14">
+        <v>1.8581367550310901</v>
+      </c>
+      <c r="N14">
+        <v>1.97281516490124</v>
+      </c>
+      <c r="O14">
+        <v>1.0049888392252599</v>
+      </c>
+      <c r="P14">
+        <v>1.8699612124614899</v>
+      </c>
+      <c r="Q14">
+        <v>1.87438170871376</v>
+      </c>
+      <c r="R14">
+        <v>1.26401272428295</v>
+      </c>
+      <c r="S14">
+        <v>2.0108186370489798</v>
+      </c>
+      <c r="T14">
+        <v>1.29265502904623</v>
+      </c>
+      <c r="U14">
+        <v>1.574607250233</v>
+      </c>
+      <c r="V14">
+        <v>1.83766488221909</v>
+      </c>
+      <c r="W14">
+        <v>2.1585004933254099</v>
+      </c>
+      <c r="X14">
+        <v>1.92757515670133</v>
+      </c>
+      <c r="Y14">
+        <v>1.8891261045457901</v>
+      </c>
+      <c r="Z14">
+        <v>1.79452568339371</v>
+      </c>
+      <c r="AA14">
+        <v>1.3803491653271101</v>
+      </c>
+      <c r="AB14">
+        <v>1.33767946103975</v>
+      </c>
+      <c r="AC14">
+        <v>2.4461672996641899</v>
+      </c>
+      <c r="AD14">
+        <v>1.0562027800228699</v>
+      </c>
+      <c r="AE14">
+        <v>1.81895677436657</v>
+      </c>
+      <c r="AF14">
+        <v>1.1374005964901499</v>
+      </c>
+      <c r="AG14">
+        <v>1.12847123350527</v>
+      </c>
+      <c r="AJ14" s="2">
+        <f t="shared" si="0"/>
+        <v>1.7179855106648354</v>
+      </c>
+      <c r="AK14" s="2">
+        <f t="shared" si="1"/>
+        <v>0.41858440716615236</v>
+      </c>
+      <c r="AL14">
+        <v>1.7179855106648354</v>
+      </c>
+    </row>
+    <row r="15" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>1.65820873146287</v>
+      </c>
+      <c r="E15">
+        <v>2.0260892231907102</v>
+      </c>
+      <c r="F15">
+        <v>2.3464172649917998</v>
+      </c>
+      <c r="G15">
+        <v>2.1156997760360001</v>
+      </c>
+      <c r="H15">
+        <v>2.0418173426678998</v>
+      </c>
+      <c r="I15">
+        <v>1.9716821644813101</v>
+      </c>
+      <c r="J15">
+        <v>1.9473396819001401</v>
+      </c>
+      <c r="K15">
+        <v>1.8958099197412599</v>
+      </c>
+      <c r="L15">
+        <v>1.46986193195633</v>
+      </c>
+      <c r="M15">
+        <v>2.9348284833042202</v>
+      </c>
+      <c r="N15">
+        <v>1.92711548689635</v>
+      </c>
+      <c r="O15">
+        <v>2.2584004046284498</v>
+      </c>
+      <c r="P15">
+        <v>2.51251097132142</v>
+      </c>
+      <c r="Q15">
+        <v>2.1295579924626198</v>
+      </c>
+      <c r="R15">
+        <v>1.8143930180764001</v>
+      </c>
+      <c r="S15">
+        <v>2.1665750835480102</v>
+      </c>
+      <c r="T15">
+        <v>2.4577187956293902</v>
+      </c>
+      <c r="U15">
+        <v>1.6523821872853599</v>
+      </c>
+      <c r="V15">
+        <v>2.4790675667848898</v>
+      </c>
+      <c r="W15">
+        <v>2.6773230126639902</v>
+      </c>
+      <c r="X15">
+        <v>2.22629480341342</v>
+      </c>
+      <c r="Y15">
+        <v>2.0667824930890402</v>
+      </c>
+      <c r="Z15">
+        <v>1.1041098487785199</v>
+      </c>
+      <c r="AA15">
+        <v>2.0869369813623702</v>
+      </c>
+      <c r="AB15">
+        <v>2.1440123388888002</v>
+      </c>
+      <c r="AC15">
+        <v>3.1826795745429601</v>
+      </c>
+      <c r="AD15">
+        <v>2.5889972483644201</v>
+      </c>
+      <c r="AE15">
+        <v>2.4337059254162599</v>
+      </c>
+      <c r="AF15">
+        <v>2.6500228667806098</v>
+      </c>
+      <c r="AG15">
+        <v>3.18549494172278</v>
+      </c>
+      <c r="AJ15" s="2">
+        <f t="shared" si="0"/>
+        <v>2.205061202046287</v>
+      </c>
+      <c r="AK15" s="2">
+        <f t="shared" si="1"/>
+        <v>0.46390893867297334</v>
+      </c>
+      <c r="AL15">
+        <v>2.205061202046287</v>
+      </c>
+    </row>
+    <row r="16" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>1.84090293081811</v>
+      </c>
+      <c r="E16">
+        <v>1.9929546844531201</v>
+      </c>
+      <c r="F16">
+        <v>0.92105962812994502</v>
+      </c>
+      <c r="G16">
+        <v>2.0289307574775801</v>
+      </c>
+      <c r="H16">
+        <v>2.5163325083497798</v>
+      </c>
+      <c r="I16">
+        <v>2.7203413119614899</v>
+      </c>
+      <c r="J16">
+        <v>2.9823404513773202</v>
+      </c>
+      <c r="K16">
+        <v>1.6886813075225899</v>
+      </c>
+      <c r="L16">
+        <v>2.6031281523068901</v>
+      </c>
+      <c r="M16">
+        <v>3.5372084802564401</v>
+      </c>
+      <c r="N16">
+        <v>1.80410718071581</v>
+      </c>
+      <c r="O16">
+        <v>1.0267362949545</v>
+      </c>
+      <c r="P16">
+        <v>1.7556576099016299</v>
+      </c>
+      <c r="Q16">
+        <v>0.88644613690859797</v>
+      </c>
+      <c r="R16">
+        <v>2.1392832727195001</v>
+      </c>
+      <c r="S16">
+        <v>0.77778440098037704</v>
+      </c>
+      <c r="T16">
+        <v>2.24918116509743</v>
+      </c>
+      <c r="U16">
+        <v>1.2557760768305199</v>
+      </c>
+      <c r="V16">
+        <v>2.6175943536955502</v>
+      </c>
+      <c r="W16">
+        <v>1.82152712894992</v>
+      </c>
+      <c r="X16">
+        <v>1.54948818773135</v>
+      </c>
+      <c r="Y16">
+        <v>2.3150106465480502</v>
+      </c>
+      <c r="Z16">
+        <v>2.9788332865987002</v>
+      </c>
+      <c r="AA16">
+        <v>0.98479722148019599</v>
+      </c>
+      <c r="AB16">
+        <v>2.2847067147316502</v>
+      </c>
+      <c r="AC16">
+        <v>2.1477010123543598</v>
+      </c>
+      <c r="AD16">
+        <v>3.12067084055658</v>
+      </c>
+      <c r="AE16">
+        <v>1.0679483650683701</v>
+      </c>
+      <c r="AF16" s="4">
+        <v>1.9924780484351701</v>
+      </c>
+      <c r="AG16">
+        <v>1.9044128532475</v>
+      </c>
+      <c r="AJ16" s="2">
+        <f t="shared" si="0"/>
+        <v>1.9837340336719673</v>
+      </c>
+      <c r="AK16" s="2">
+        <f t="shared" si="1"/>
+        <v>0.72187381564627606</v>
+      </c>
+      <c r="AL16">
+        <v>1.9837340336719673</v>
+      </c>
+      <c r="AO16" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP16" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ16" t="s">
+        <v>7</v>
+      </c>
+      <c r="AR16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AS16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>4.0301837340595004</v>
+      </c>
+      <c r="E17">
+        <v>2.1916244955737598</v>
+      </c>
+      <c r="F17">
+        <v>2.4315097797033101</v>
+      </c>
+      <c r="G17">
+        <v>3.9658948484845302</v>
+      </c>
+      <c r="H17">
+        <v>1.30282399925017</v>
+      </c>
+      <c r="I17">
+        <v>2.36996951711185</v>
+      </c>
+      <c r="J17">
+        <v>1.97170034443066</v>
+      </c>
+      <c r="K17">
+        <v>1.8485782691830701</v>
+      </c>
+      <c r="L17">
+        <v>1.42193504041995</v>
+      </c>
+      <c r="M17">
+        <v>2.6009046264066198</v>
+      </c>
+      <c r="N17">
+        <v>1.5569900954871401</v>
+      </c>
+      <c r="O17">
+        <v>2.4398987859329</v>
+      </c>
+      <c r="P17">
+        <v>2.82096973102708</v>
+      </c>
+      <c r="Q17">
+        <v>1.1539376363687699</v>
+      </c>
+      <c r="R17">
+        <v>0.91294074283663396</v>
+      </c>
+      <c r="S17">
+        <v>1.5750342311152501</v>
+      </c>
+      <c r="T17">
+        <v>2.7378582197195098</v>
+      </c>
+      <c r="U17">
+        <v>3.2407783802015202</v>
+      </c>
+      <c r="V17">
+        <v>2.44048849899134</v>
+      </c>
+      <c r="W17">
+        <v>1.38576334456971</v>
+      </c>
+      <c r="X17">
+        <v>3.2317492118818998</v>
+      </c>
+      <c r="Y17">
+        <v>1.8324875764298201</v>
+      </c>
+      <c r="Z17">
+        <v>2.4192412810245298</v>
+      </c>
+      <c r="AA17">
+        <v>2.5327474680863098</v>
+      </c>
+      <c r="AB17">
+        <v>1.5788077000052301</v>
+      </c>
+      <c r="AC17">
+        <v>1.5810440342871701</v>
+      </c>
+      <c r="AD17">
+        <v>2.0826471075198598</v>
+      </c>
+      <c r="AE17">
+        <v>2.32175640863495</v>
+      </c>
+      <c r="AF17">
+        <v>2.9812026752987801</v>
+      </c>
+      <c r="AG17">
+        <v>3.5807310232991099</v>
+      </c>
+      <c r="AJ17" s="2">
+        <f t="shared" si="0"/>
+        <v>2.2847399602446976</v>
+      </c>
+      <c r="AK17" s="2">
+        <f t="shared" si="1"/>
+        <v>0.80613321458593534</v>
+      </c>
+      <c r="AL17">
+        <v>2.2847399602446976</v>
+      </c>
+      <c r="AO17">
+        <v>5</v>
+      </c>
+      <c r="AP17">
+        <v>1.6150663743236735</v>
+      </c>
+      <c r="AQ17">
+        <v>2.1562636783693474</v>
+      </c>
+      <c r="AR17">
+        <v>1.6690253864999696</v>
+      </c>
+      <c r="AS17">
+        <v>2.0841411531572165</v>
+      </c>
+    </row>
+    <row r="18" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AF18" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ18" s="2"/>
+      <c r="AK18" s="2"/>
+      <c r="AO18">
+        <v>10</v>
+      </c>
+      <c r="AP18">
+        <v>3.4727194131047758</v>
+      </c>
+      <c r="AQ18">
+        <v>4.6203290330256275</v>
+      </c>
+      <c r="AR18">
+        <v>3.8604717711463024</v>
+      </c>
+      <c r="AS18">
+        <v>4.7214033657582339</v>
+      </c>
+    </row>
+    <row r="19" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AF19" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK19" s="2"/>
+      <c r="AO19">
+        <v>20</v>
+      </c>
+      <c r="AP19">
+        <v>4.825152644366649</v>
+      </c>
+      <c r="AQ19">
+        <v>8.1297108955336537</v>
+      </c>
+      <c r="AR19">
+        <v>5.7203499395237367</v>
+      </c>
+      <c r="AS19">
+        <v>8.7698047774647314</v>
+      </c>
+    </row>
+    <row r="20" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>4.0756123916889297</v>
+      </c>
+      <c r="E20">
+        <v>2.9542893805674599</v>
+      </c>
+      <c r="F20">
+        <v>3.4105919248692498</v>
+      </c>
+      <c r="G20">
+        <v>3.9373318706162501</v>
+      </c>
+      <c r="H20">
+        <v>3.2180589245726101</v>
+      </c>
+      <c r="I20">
+        <v>2.6761933091914498</v>
+      </c>
+      <c r="J20">
+        <v>3.5040001321258401</v>
+      </c>
+      <c r="K20">
+        <v>3.9913191913320101</v>
+      </c>
+      <c r="L20">
+        <v>3.3996030660363599</v>
+      </c>
+      <c r="M20">
+        <v>3.4427340464195599</v>
+      </c>
+      <c r="N20">
+        <v>3.2782727147617501</v>
+      </c>
+      <c r="O20">
+        <v>4.0125115766828596</v>
+      </c>
+      <c r="P20">
+        <v>3.3797053668188299</v>
+      </c>
+      <c r="Q20">
+        <v>4.0030034899241604</v>
+      </c>
+      <c r="R20">
+        <v>3.8487982993453298</v>
+      </c>
+      <c r="S20">
+        <v>4.4658125871423104</v>
+      </c>
+      <c r="T20">
+        <v>3.2979919773297599</v>
+      </c>
+      <c r="U20">
+        <v>3.61193695098354</v>
+      </c>
+      <c r="V20">
+        <v>3.10845766527085</v>
+      </c>
+      <c r="W20">
+        <v>3.8886177289693999</v>
+      </c>
+      <c r="X20">
+        <v>4.0440336170156002</v>
+      </c>
+      <c r="Y20">
+        <v>2.2225464182607002</v>
+      </c>
+      <c r="Z20">
+        <v>2.6325289316753202</v>
+      </c>
+      <c r="AA20">
+        <v>3.1381672959533802</v>
+      </c>
+      <c r="AB20">
+        <v>3.1385222013048701</v>
+      </c>
+      <c r="AC20">
+        <v>3.5688271194044998</v>
+      </c>
+      <c r="AD20">
+        <v>4.1487948538763701</v>
+      </c>
+      <c r="AE20">
+        <v>3.6863068820499501</v>
+      </c>
+      <c r="AF20">
+        <v>3.2996756458298502</v>
+      </c>
+      <c r="AG20">
+        <v>2.7973368331242199</v>
+      </c>
+      <c r="AJ20" s="2">
+        <f t="shared" ref="AJ20:AL35" si="2">AVERAGE(D20:AG20)</f>
+        <v>3.4727194131047758</v>
+      </c>
+      <c r="AK20" s="2">
+        <f t="shared" ref="AK20:AK35" si="3">_xlfn.STDEV.S(D20:AG20)</f>
+        <v>0.51684091172016056</v>
+      </c>
+      <c r="AL20">
+        <v>3.4727194131047758</v>
+      </c>
+    </row>
+    <row r="21" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>5.5531444969208001</v>
+      </c>
+      <c r="E21">
+        <v>3.57973764878879</v>
+      </c>
+      <c r="F21">
+        <v>4.2596772755712298</v>
+      </c>
+      <c r="G21">
+        <v>5.06608794646273</v>
+      </c>
+      <c r="H21">
+        <v>5.87850258189901</v>
+      </c>
+      <c r="I21">
+        <v>3.7208641566987302</v>
+      </c>
+      <c r="J21">
+        <v>5.6451989425406701</v>
+      </c>
+      <c r="K21">
+        <v>4.4271728919337301</v>
+      </c>
+      <c r="L21">
+        <v>4.2037291621390596</v>
+      </c>
+      <c r="M21">
+        <v>4.1602147528762199</v>
+      </c>
+      <c r="N21">
+        <v>4.0394470797495998</v>
+      </c>
+      <c r="O21">
+        <v>4.7226740532968101</v>
+      </c>
+      <c r="P21">
+        <v>5.7313230384257299</v>
+      </c>
+      <c r="Q21">
+        <v>3.07801076504823</v>
+      </c>
+      <c r="R21">
+        <v>3.5826137607817201</v>
+      </c>
+      <c r="S21">
+        <v>3.7498275858455199</v>
+      </c>
+      <c r="T21">
+        <v>5.7096083909727602</v>
+      </c>
+      <c r="U21">
+        <v>3.00957318927022</v>
+      </c>
+      <c r="V21">
+        <v>4.6768456741230304</v>
+      </c>
+      <c r="W21">
+        <v>5.2749074411932204</v>
+      </c>
+      <c r="X21">
+        <v>3.7912272732522201</v>
+      </c>
+      <c r="Y21">
+        <v>4.1958415949747199</v>
+      </c>
+      <c r="Z21">
+        <v>4.35319892010651</v>
+      </c>
+      <c r="AA21">
+        <v>4.1218412015825496</v>
+      </c>
+      <c r="AB21">
+        <v>5.2319962828886197</v>
+      </c>
+      <c r="AC21">
+        <v>5.5831627364818202</v>
+      </c>
+      <c r="AD21">
+        <v>5.64440004982949</v>
+      </c>
+      <c r="AE21">
+        <v>4.5117733698020102</v>
+      </c>
+      <c r="AF21">
+        <v>5.9002292635845901</v>
+      </c>
+      <c r="AG21">
+        <v>5.2070394637284902</v>
+      </c>
+      <c r="AJ21" s="2">
+        <f t="shared" si="2"/>
+        <v>4.6203290330256275</v>
+      </c>
+      <c r="AK21" s="2">
+        <f t="shared" si="3"/>
+        <v>0.86476094257046399</v>
+      </c>
+      <c r="AL21">
+        <v>4.6203290330256275</v>
+      </c>
+    </row>
+    <row r="22" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>2.9565179421134098</v>
+      </c>
+      <c r="E22">
+        <v>4.2521211432961099</v>
+      </c>
+      <c r="F22">
+        <v>3.7624717891294499</v>
+      </c>
+      <c r="G22">
+        <v>3.6146664571679299</v>
+      </c>
+      <c r="H22">
+        <v>3.3419734916839499</v>
+      </c>
+      <c r="I22">
+        <v>3.5266533759168199</v>
+      </c>
+      <c r="J22">
+        <v>4.44020162997219</v>
+      </c>
+      <c r="K22">
+        <v>4.4878694418021796</v>
+      </c>
+      <c r="L22">
+        <v>4.1023408921970503</v>
+      </c>
+      <c r="M22">
+        <v>4.0150115066207697</v>
+      </c>
+      <c r="N22">
+        <v>4.2360488901011299</v>
+      </c>
+      <c r="O22">
+        <v>4.8714425555276799</v>
+      </c>
+      <c r="P22">
+        <v>4.0513954487165602</v>
+      </c>
+      <c r="Q22">
+        <v>3.7283015308245799</v>
+      </c>
+      <c r="R22">
+        <v>4.4193360946673002</v>
+      </c>
+      <c r="S22">
+        <v>3.10032031841933</v>
+      </c>
+      <c r="T22">
+        <v>3.1436823455314098</v>
+      </c>
+      <c r="U22">
+        <v>3.6574996438534702</v>
+      </c>
+      <c r="V22">
+        <v>3.8333860804575299</v>
+      </c>
+      <c r="W22">
+        <v>3.6584430553417202</v>
+      </c>
+      <c r="X22">
+        <v>3.6188662543179402</v>
+      </c>
+      <c r="Y22">
+        <v>2.8419917590516599</v>
+      </c>
+      <c r="Z22">
+        <v>4.6070287242010499</v>
+      </c>
+      <c r="AA22">
+        <v>4.4706642481203103</v>
+      </c>
+      <c r="AB22">
+        <v>3.5877929006396898</v>
+      </c>
+      <c r="AC22">
+        <v>2.95941790599738</v>
+      </c>
+      <c r="AD22">
+        <v>3.1092508550778502</v>
+      </c>
+      <c r="AE22">
+        <v>4.3032991784302101</v>
+      </c>
+      <c r="AF22">
+        <v>4.7069164733269098</v>
+      </c>
+      <c r="AG22">
+        <v>4.4092412018855001</v>
+      </c>
+      <c r="AJ22" s="2">
+        <f t="shared" si="2"/>
+        <v>3.8604717711463024</v>
+      </c>
+      <c r="AK22" s="2">
+        <f t="shared" si="3"/>
+        <v>0.57614376989512062</v>
+      </c>
+      <c r="AL22">
+        <v>3.8604717711463024</v>
+      </c>
+      <c r="AO22" t="s">
+        <v>29</v>
+      </c>
+      <c r="AP22" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ22" t="s">
+        <v>7</v>
+      </c>
+      <c r="AR22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AS22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>5.8585941567356601</v>
+      </c>
+      <c r="E23">
+        <v>4.0554320455072999</v>
+      </c>
+      <c r="F23">
+        <v>4.4686284704327397</v>
+      </c>
+      <c r="G23">
+        <v>4.3161087469203698</v>
+      </c>
+      <c r="H23">
+        <v>4.07505440537577</v>
+      </c>
+      <c r="I23">
+        <v>4.3448715686801096</v>
+      </c>
+      <c r="J23">
+        <v>4.8026466088316102</v>
+      </c>
+      <c r="K23">
+        <v>4.7848536372931196</v>
+      </c>
+      <c r="L23">
+        <v>4.7541592295024397</v>
+      </c>
+      <c r="M23">
+        <v>4.7074221543546599</v>
+      </c>
+      <c r="N23">
+        <v>4.8807199824552399</v>
+      </c>
+      <c r="O23">
+        <v>4.3995658868719403</v>
+      </c>
+      <c r="P23">
+        <v>5.4728262872016096</v>
+      </c>
+      <c r="Q23">
+        <v>4.8146020702996397</v>
+      </c>
+      <c r="R23">
+        <v>4.5705297983189404</v>
+      </c>
+      <c r="S23">
+        <v>3.82537702548822</v>
+      </c>
+      <c r="T23">
+        <v>5.4538364265074604</v>
+      </c>
+      <c r="U23">
+        <v>5.2695357213099001</v>
+      </c>
+      <c r="V23">
+        <v>4.7126256819048304</v>
+      </c>
+      <c r="W23">
+        <v>4.2490308560562404</v>
+      </c>
+      <c r="X23">
+        <v>3.2835583578388499</v>
+      </c>
+      <c r="Y23">
+        <v>4.1754455964183101</v>
+      </c>
+      <c r="Z23">
+        <v>4.1677501313949801</v>
+      </c>
+      <c r="AA23">
+        <v>4.5443185689875598</v>
+      </c>
+      <c r="AB23">
+        <v>5.6759841169122396</v>
+      </c>
+      <c r="AC23">
+        <v>6.1826715449504297</v>
+      </c>
+      <c r="AD23">
+        <v>4.4912035591168404</v>
+      </c>
+      <c r="AE23">
+        <v>6.3519185402292999</v>
+      </c>
+      <c r="AF23">
+        <v>4.0975853604766099</v>
+      </c>
+      <c r="AG23">
+        <v>4.8552444363740896</v>
+      </c>
+      <c r="AJ23" s="2">
+        <f t="shared" si="2"/>
+        <v>4.7214033657582339</v>
+      </c>
+      <c r="AK23" s="2">
+        <f t="shared" si="3"/>
+        <v>0.6946313699158696</v>
+      </c>
+      <c r="AL23">
+        <v>4.7214033657582339</v>
+      </c>
+      <c r="AO23">
+        <v>5</v>
+      </c>
+      <c r="AP23">
+        <v>1.7179855106648354</v>
+      </c>
+      <c r="AQ23">
+        <v>2.205061202046287</v>
+      </c>
+      <c r="AR23">
+        <v>1.9837340336719673</v>
+      </c>
+      <c r="AS23">
+        <v>2.2847399602446976</v>
+      </c>
+    </row>
+    <row r="24" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AF24" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI24" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ24" s="2"/>
+      <c r="AK24" s="2"/>
+      <c r="AO24">
+        <v>10</v>
+      </c>
+      <c r="AP24">
+        <v>3.8197596205068676</v>
+      </c>
+      <c r="AQ24">
+        <v>4.6782716422325175</v>
+      </c>
+      <c r="AR24">
+        <v>5.5650747070751079</v>
+      </c>
+      <c r="AS24">
+        <v>5.4250457018306415</v>
+      </c>
+    </row>
+    <row r="25" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AF25" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI25" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK25" s="2"/>
+      <c r="AO25">
+        <v>20</v>
+      </c>
+      <c r="AP25">
+        <v>6.1724764986002869</v>
+      </c>
+      <c r="AQ25">
+        <v>9.4669736430625715</v>
+      </c>
+      <c r="AR25">
+        <v>9.6695592331222908</v>
+      </c>
+      <c r="AS25">
+        <v>11.457843891273024</v>
+      </c>
+    </row>
+    <row r="26" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>2.7378164797915399</v>
+      </c>
+      <c r="E26">
+        <v>3.3472059779421599</v>
+      </c>
+      <c r="F26">
+        <v>5.1154124276810897</v>
+      </c>
+      <c r="G26">
+        <v>4.2921712943999903</v>
+      </c>
+      <c r="H26">
+        <v>2.9689813141660499</v>
+      </c>
+      <c r="I26">
+        <v>2.5136881519004599</v>
+      </c>
+      <c r="J26">
+        <v>3.9000024310277102</v>
+      </c>
+      <c r="K26">
+        <v>4.1979367251610098</v>
+      </c>
+      <c r="L26">
+        <v>4.4845582363938101</v>
+      </c>
+      <c r="M26">
+        <v>3.8692764356140699</v>
+      </c>
+      <c r="N26">
+        <v>3.1599205140131499</v>
+      </c>
+      <c r="O26">
+        <v>4.23286472795054</v>
+      </c>
+      <c r="P26">
+        <v>4.1218347938417299</v>
+      </c>
+      <c r="Q26">
+        <v>4.1938158892592803</v>
+      </c>
+      <c r="R26">
+        <v>4.0929520216787303</v>
+      </c>
+      <c r="S26">
+        <v>3.4393771838335399</v>
+      </c>
+      <c r="T26">
+        <v>4.1575213977489298</v>
+      </c>
+      <c r="U26">
+        <v>3.7747632770411701</v>
+      </c>
+      <c r="V26">
+        <v>4.0868975746094804</v>
+      </c>
+      <c r="W26">
+        <v>4.3254683498601203</v>
+      </c>
+      <c r="X26">
+        <v>2.9923380106283402</v>
+      </c>
+      <c r="Y26">
+        <v>3.5497452173254902</v>
+      </c>
+      <c r="Z26">
+        <v>3.35593882832667</v>
+      </c>
+      <c r="AA26">
+        <v>3.6233654490568701</v>
+      </c>
+      <c r="AB26">
+        <v>4.7205352019415701</v>
+      </c>
+      <c r="AC26">
+        <v>3.4965016689622099</v>
+      </c>
+      <c r="AD26">
+        <v>4.0836026430737702</v>
+      </c>
+      <c r="AE26">
+        <v>4.24044991127065</v>
+      </c>
+      <c r="AF26">
+        <v>3.6401275482243101</v>
+      </c>
+      <c r="AG26">
+        <v>3.87771893248157</v>
+      </c>
+      <c r="AJ26" s="2">
+        <f t="shared" si="2"/>
+        <v>3.8197596205068676</v>
+      </c>
+      <c r="AK26" s="2">
+        <f t="shared" si="3"/>
+        <v>0.58805360640950222</v>
+      </c>
+      <c r="AL26">
+        <v>3.8197596205068676</v>
+      </c>
+    </row>
+    <row r="27" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>4.6923235051243903</v>
+      </c>
+      <c r="E27">
+        <v>2.6666052493540899</v>
+      </c>
+      <c r="F27">
+        <v>5.1123108843664102</v>
+      </c>
+      <c r="G27">
+        <v>3.0617586091603401</v>
+      </c>
+      <c r="H27">
+        <v>6.3453743840241197</v>
+      </c>
+      <c r="I27">
+        <v>3.5991409236778198</v>
+      </c>
+      <c r="J27">
+        <v>4.7546129422020398</v>
+      </c>
+      <c r="K27">
+        <v>4.93452860346944</v>
+      </c>
+      <c r="L27">
+        <v>4.6375720758760899</v>
+      </c>
+      <c r="M27">
+        <v>4.9920624201583603</v>
+      </c>
+      <c r="N27">
+        <v>4.2887107879781103</v>
+      </c>
+      <c r="O27">
+        <v>4.7158800432709098</v>
+      </c>
+      <c r="P27">
+        <v>5.3126721537631001</v>
+      </c>
+      <c r="Q27">
+        <v>4.5353007125345197</v>
+      </c>
+      <c r="R27">
+        <v>3.9972236920445301</v>
+      </c>
+      <c r="S27">
+        <v>4.0312231034754697</v>
+      </c>
+      <c r="T27">
+        <v>4.9857959090324204</v>
+      </c>
+      <c r="U27">
+        <v>4.4910789904858799</v>
+      </c>
+      <c r="V27">
+        <v>5.3891352115469502</v>
+      </c>
+      <c r="W27">
+        <v>5.5726009973119996</v>
+      </c>
+      <c r="X27">
+        <v>4.3021227265280304</v>
+      </c>
+      <c r="Y27">
+        <v>4.1338635934709904</v>
+      </c>
+      <c r="Z27">
+        <v>4.5998650069830402</v>
+      </c>
+      <c r="AA27">
+        <v>3.71971753309895</v>
+      </c>
+      <c r="AB27">
+        <v>4.7032644447243701</v>
+      </c>
+      <c r="AC27">
+        <v>7.5294267954459597</v>
+      </c>
+      <c r="AD27">
+        <v>4.21194700372748</v>
+      </c>
+      <c r="AE27">
+        <v>4.5757155063708499</v>
+      </c>
+      <c r="AF27">
+        <v>5.4338062950661499</v>
+      </c>
+      <c r="AG27">
+        <v>5.02250916270276</v>
+      </c>
+      <c r="AJ27" s="2">
+        <f t="shared" si="2"/>
+        <v>4.6782716422325175</v>
+      </c>
+      <c r="AK27" s="2">
+        <f t="shared" si="3"/>
+        <v>0.9147653681418928</v>
+      </c>
+      <c r="AL27">
+        <v>4.6782716422325175</v>
+      </c>
+    </row>
+    <row r="28" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>8.7978431895031903</v>
+      </c>
+      <c r="E28">
+        <v>4.7338869246335902</v>
+      </c>
+      <c r="F28">
+        <v>4.5360868658280102</v>
+      </c>
+      <c r="G28">
+        <v>5.2974164744512997</v>
+      </c>
+      <c r="H28">
+        <v>3.9380174942729198</v>
+      </c>
+      <c r="I28">
+        <v>4.0692009396038298</v>
+      </c>
+      <c r="J28">
+        <v>4.8229408417086699</v>
+      </c>
+      <c r="K28">
+        <v>4.6638675175916804</v>
+      </c>
+      <c r="L28">
+        <v>6.0649229220804699</v>
+      </c>
+      <c r="M28">
+        <v>6.3574030116906401</v>
+      </c>
+      <c r="N28">
+        <v>6.7255698535496196</v>
+      </c>
+      <c r="O28">
+        <v>8.3350819866362595</v>
+      </c>
+      <c r="P28">
+        <v>5.3977217898756802</v>
+      </c>
+      <c r="Q28">
+        <v>6.0453820015905002</v>
+      </c>
+      <c r="R28">
+        <v>6.1179568743910204</v>
+      </c>
+      <c r="S28">
+        <v>4.3942427423996602</v>
+      </c>
+      <c r="T28">
+        <v>3.51965454626378</v>
+      </c>
+      <c r="U28">
+        <v>5.7296781829493302</v>
+      </c>
+      <c r="V28">
+        <v>3.5931300218654099</v>
+      </c>
+      <c r="W28">
+        <v>7.2013254180558501</v>
+      </c>
+      <c r="X28">
+        <v>5.1674408394213396</v>
+      </c>
+      <c r="Y28">
+        <v>7.0618188567026898</v>
+      </c>
+      <c r="Z28">
+        <v>5.93182122830481</v>
+      </c>
+      <c r="AA28">
+        <v>7.1150649310129701</v>
+      </c>
+      <c r="AB28">
+        <v>5.1814695669568103</v>
+      </c>
+      <c r="AC28">
+        <v>8.6704816700547003</v>
+      </c>
+      <c r="AD28">
+        <v>3.2889106203508498</v>
+      </c>
+      <c r="AE28">
+        <v>3.9618317150895099</v>
+      </c>
+      <c r="AF28" s="4">
+        <v>4.6516291722660403</v>
+      </c>
+      <c r="AG28">
+        <v>5.5804430131520899</v>
+      </c>
+      <c r="AJ28" s="2">
+        <f t="shared" si="2"/>
+        <v>5.5650747070751079</v>
+      </c>
+      <c r="AK28" s="2">
+        <f t="shared" si="3"/>
+        <v>1.4906749979905278</v>
+      </c>
+      <c r="AL28">
+        <v>5.5650747070751079</v>
+      </c>
+    </row>
+    <row r="29" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>5.62575630171421</v>
+      </c>
+      <c r="E29">
+        <v>3.8854678766225899</v>
+      </c>
+      <c r="F29">
+        <v>2.4755270349406699</v>
+      </c>
+      <c r="G29">
+        <v>5.6862171502679999</v>
+      </c>
+      <c r="H29">
+        <v>6.1315350077386004</v>
+      </c>
+      <c r="I29">
+        <v>6.9492301993341696</v>
+      </c>
+      <c r="J29">
+        <v>6.0491400852590997</v>
+      </c>
+      <c r="K29">
+        <v>5.5864906892668902</v>
+      </c>
+      <c r="L29">
+        <v>7.4134391770468504</v>
+      </c>
+      <c r="M29">
+        <v>4.5306687119713596</v>
+      </c>
+      <c r="N29">
+        <v>8.1279090759184101</v>
+      </c>
+      <c r="O29">
+        <v>4.3622728220248197</v>
+      </c>
+      <c r="P29">
+        <v>5.0556227375131497</v>
+      </c>
+      <c r="Q29">
+        <v>15.164863636104201</v>
+      </c>
+      <c r="R29">
+        <v>5.1470530812040201</v>
+      </c>
+      <c r="S29">
+        <v>5.5482098533364796</v>
+      </c>
+      <c r="T29">
+        <v>8.1577468663239898</v>
+      </c>
+      <c r="U29">
+        <v>10.867684419273401</v>
+      </c>
+      <c r="V29">
+        <v>4.1015157814874001</v>
+      </c>
+      <c r="W29">
+        <v>3.2814004898242102</v>
+      </c>
+      <c r="X29">
+        <v>5.2680626487787103</v>
+      </c>
+      <c r="Y29">
+        <v>3.3507067754828102</v>
+      </c>
+      <c r="Z29">
+        <v>1.6787980771391899</v>
+      </c>
+      <c r="AA29">
+        <v>3.4307719283149201</v>
+      </c>
+      <c r="AB29">
+        <v>4.0989043259922804</v>
+      </c>
+      <c r="AC29">
+        <v>3.41779113347414</v>
+      </c>
+      <c r="AD29">
+        <v>4.9663833277879803</v>
+      </c>
+      <c r="AE29">
+        <v>4.2295542540314397</v>
+      </c>
+      <c r="AF29">
+        <v>6.1580501566387902</v>
+      </c>
+      <c r="AG29">
+        <v>2.00459743010647</v>
+      </c>
+      <c r="AJ29" s="2">
+        <f t="shared" si="2"/>
+        <v>5.4250457018306415</v>
+      </c>
+      <c r="AK29" s="2">
+        <f t="shared" si="3"/>
+        <v>2.6790234223384064</v>
+      </c>
+      <c r="AL29">
+        <v>5.4250457018306415</v>
+      </c>
+    </row>
+    <row r="30" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AF30" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI30" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ30" s="2"/>
+      <c r="AK30" s="2"/>
+    </row>
+    <row r="31" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AF31" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI31" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK31" s="2"/>
+    </row>
+    <row r="32" spans="4:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>6.1815207076885903</v>
+      </c>
+      <c r="E32">
+        <v>5.3315172765683201</v>
+      </c>
+      <c r="F32">
+        <v>5.6636039962810196</v>
+      </c>
+      <c r="G32">
+        <v>2.01777988514969</v>
+      </c>
+      <c r="H32">
+        <v>5.5029403274881297</v>
+      </c>
+      <c r="I32">
+        <v>5.60084998402065</v>
+      </c>
+      <c r="J32">
+        <v>4.6275325668429499</v>
+      </c>
+      <c r="K32">
+        <v>2.0937407931360399</v>
+      </c>
+      <c r="L32">
+        <v>5.6434477856051402</v>
+      </c>
+      <c r="M32">
+        <v>4.7182910981136503</v>
+      </c>
+      <c r="N32">
+        <v>5.2826505365649998</v>
+      </c>
+      <c r="O32">
+        <v>3.2761988361059999</v>
+      </c>
+      <c r="P32">
+        <v>3.42364087664185</v>
+      </c>
+      <c r="Q32">
+        <v>5.43033431905888</v>
+      </c>
+      <c r="R32">
+        <v>6.5682685560503096</v>
+      </c>
+      <c r="S32">
+        <v>5.30426230823615</v>
+      </c>
+      <c r="T32">
+        <v>4.2474631011713804</v>
+      </c>
+      <c r="U32">
+        <v>6.32017559385715</v>
+      </c>
+      <c r="V32">
+        <v>6.07421835171428</v>
+      </c>
+      <c r="W32">
+        <v>3.55248002960565</v>
+      </c>
+      <c r="X32">
+        <v>4.8239727874768397</v>
+      </c>
+      <c r="Y32">
+        <v>4.2550978394219996</v>
+      </c>
+      <c r="Z32">
+        <v>5.5950658599250804</v>
+      </c>
+      <c r="AA32">
+        <v>4.9400793031106902</v>
+      </c>
+      <c r="AB32">
+        <v>6.1465729640617299</v>
+      </c>
+      <c r="AC32">
+        <v>3.7677791771429399</v>
+      </c>
+      <c r="AD32">
+        <v>6.0053401544347702</v>
+      </c>
+      <c r="AE32">
+        <v>5.0165219382086104</v>
+      </c>
+      <c r="AF32">
+        <v>3.8289595495810298</v>
+      </c>
+      <c r="AG32">
+        <v>3.51427282773495</v>
+      </c>
+      <c r="AJ32" s="2">
+        <f t="shared" si="2"/>
+        <v>4.825152644366649</v>
+      </c>
+      <c r="AK32" s="2">
+        <f t="shared" si="3"/>
+        <v>1.2007669419135463</v>
+      </c>
+      <c r="AL32">
+        <v>4.825152644366649</v>
+      </c>
+    </row>
+    <row r="33" spans="4:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>9.9008391262143007</v>
+      </c>
+      <c r="E33">
+        <v>9.3503129327298993</v>
+      </c>
+      <c r="F33">
+        <v>8.7944012277640908</v>
+      </c>
+      <c r="G33">
+        <v>8.0070228101851999</v>
+      </c>
+      <c r="H33">
+        <v>7.3649083380142102</v>
+      </c>
+      <c r="I33">
+        <v>5.3053187309962198</v>
+      </c>
+      <c r="J33">
+        <v>9.4930904083448198</v>
+      </c>
+      <c r="K33">
+        <v>5.1504679938671902</v>
+      </c>
+      <c r="L33">
+        <v>5.8887382723442601</v>
+      </c>
+      <c r="M33">
+        <v>10.4449286274922</v>
+      </c>
+      <c r="N33">
+        <v>5.8569945628367197</v>
+      </c>
+      <c r="O33">
+        <v>11.238460787620999</v>
+      </c>
+      <c r="P33">
+        <v>7.7060590205114803</v>
+      </c>
+      <c r="Q33">
+        <v>9.3575006780337997</v>
+      </c>
+      <c r="R33">
+        <v>8.4405371357539298</v>
+      </c>
+      <c r="S33">
+        <v>6.6984669474216902</v>
+      </c>
+      <c r="T33">
+        <v>10.082159434948901</v>
+      </c>
+      <c r="U33">
+        <v>8.5551231713772697</v>
+      </c>
+      <c r="V33">
+        <v>7.3957562412047899</v>
+      </c>
+      <c r="W33">
+        <v>8.3173784707603904</v>
+      </c>
+      <c r="X33">
+        <v>8.1102193313597599</v>
+      </c>
+      <c r="Y33">
+        <v>7.73321768197835</v>
+      </c>
+      <c r="Z33">
+        <v>7.703747426704</v>
+      </c>
+      <c r="AA33">
+        <v>6.7331728940358104</v>
+      </c>
+      <c r="AB33">
+        <v>7.0447109584365997</v>
+      </c>
+      <c r="AC33">
+        <v>9.9556535915671702</v>
+      </c>
+      <c r="AD33">
+        <v>7.2095312044198598</v>
+      </c>
+      <c r="AE33">
+        <v>10.0480253219266</v>
+      </c>
+      <c r="AF33">
+        <v>8.3620765462583595</v>
+      </c>
+      <c r="AG33">
+        <v>7.6425069909007597</v>
+      </c>
+      <c r="AJ33" s="2">
+        <f t="shared" si="2"/>
+        <v>8.1297108955336537</v>
+      </c>
+      <c r="AK33" s="2">
+        <f t="shared" si="3"/>
+        <v>1.5493025942255869</v>
+      </c>
+      <c r="AL33">
+        <v>8.1297108955336537</v>
+      </c>
+    </row>
+    <row r="34" spans="4:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>5.2330195154598496</v>
+      </c>
+      <c r="E34">
+        <v>6.1622472428951598</v>
+      </c>
+      <c r="F34">
+        <v>5.4248897258197299</v>
+      </c>
+      <c r="G34">
+        <v>5.5897683900887296</v>
+      </c>
+      <c r="H34">
+        <v>5.6268195833503603</v>
+      </c>
+      <c r="I34">
+        <v>4.7419826735460804</v>
+      </c>
+      <c r="J34">
+        <v>6.6918794435812403</v>
+      </c>
+      <c r="K34">
+        <v>6.3525034529091204</v>
+      </c>
+      <c r="L34">
+        <v>4.5302347251225301</v>
+      </c>
+      <c r="M34">
+        <v>6.1432121395511601</v>
+      </c>
+      <c r="N34">
+        <v>5.3199199402533699</v>
+      </c>
+      <c r="O34">
+        <v>7.13959670279303</v>
+      </c>
+      <c r="P34">
+        <v>4.5426624533911397</v>
+      </c>
+      <c r="Q34">
+        <v>7.0652626526056803</v>
+      </c>
+      <c r="R34">
+        <v>6.8316252067693197</v>
+      </c>
+      <c r="S34">
+        <v>5.1624295986008804</v>
+      </c>
+      <c r="T34">
+        <v>5.2241921894121699</v>
+      </c>
+      <c r="U34">
+        <v>5.4441641433941799</v>
+      </c>
+      <c r="V34">
+        <v>6.3065519477626699</v>
+      </c>
+      <c r="W34">
+        <v>5.4580932267464899</v>
+      </c>
+      <c r="X34">
+        <v>4.0018807341689202</v>
+      </c>
+      <c r="Y34">
+        <v>5.6909592086229104</v>
+      </c>
+      <c r="Z34">
+        <v>6.4089232021691798</v>
+      </c>
+      <c r="AA34">
+        <v>4.0763986705885298</v>
+      </c>
+      <c r="AB34">
+        <v>6.3397243135870101</v>
+      </c>
+      <c r="AC34">
+        <v>4.9659273551828296</v>
+      </c>
+      <c r="AD34">
+        <v>6.70087916137207</v>
+      </c>
+      <c r="AE34">
+        <v>5.4313151579203902</v>
+      </c>
+      <c r="AF34">
+        <v>6.4808059028547298</v>
+      </c>
+      <c r="AG34">
+        <v>6.5226295251926496</v>
+      </c>
+      <c r="AJ34" s="2">
+        <f t="shared" si="2"/>
+        <v>5.7203499395237367</v>
+      </c>
+      <c r="AK34" s="2">
+        <f t="shared" si="3"/>
+        <v>0.85990301645553247</v>
+      </c>
+      <c r="AL34">
+        <v>5.7203499395237367</v>
+      </c>
+    </row>
+    <row r="35" spans="4:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>9.4521866865593207</v>
+      </c>
+      <c r="E35">
+        <v>8.2189788059576596</v>
+      </c>
+      <c r="F35">
+        <v>9.9194483477066395</v>
+      </c>
+      <c r="G35">
+        <v>9.0061231464709497</v>
+      </c>
+      <c r="H35">
+        <v>9.5773423359620597</v>
+      </c>
+      <c r="I35">
+        <v>3.9016062261018898</v>
+      </c>
+      <c r="J35">
+        <v>7.9805002994240004</v>
+      </c>
+      <c r="K35">
+        <v>11.708455636414101</v>
+      </c>
+      <c r="L35">
+        <v>10.8263643832752</v>
+      </c>
+      <c r="M35">
+        <v>9.3016903994538893</v>
+      </c>
+      <c r="N35">
+        <v>9.5214316913846098</v>
+      </c>
+      <c r="O35">
+        <v>13.0392175722794</v>
+      </c>
+      <c r="P35">
+        <v>11.5755077506014</v>
+      </c>
+      <c r="Q35">
+        <v>7.4623636261930297</v>
+      </c>
+      <c r="R35">
+        <v>7.2366080256313099</v>
+      </c>
+      <c r="S35">
+        <v>8.2074757726823293</v>
+      </c>
+      <c r="T35">
+        <v>9.88646158453823</v>
+      </c>
+      <c r="U35">
+        <v>7.9092272217919204</v>
+      </c>
+      <c r="V35">
+        <v>9.1086780792916695</v>
+      </c>
+      <c r="W35">
+        <v>10.8905905382427</v>
+      </c>
+      <c r="X35">
+        <v>7.3987968161950199</v>
+      </c>
+      <c r="Y35">
+        <v>6.9689789579697203</v>
+      </c>
+      <c r="Z35">
+        <v>6.9452805239246196</v>
+      </c>
+      <c r="AA35">
+        <v>8.9229587417429901</v>
+      </c>
+      <c r="AB35">
+        <v>10.1483942102114</v>
+      </c>
+      <c r="AC35">
+        <v>8.6778627458421802</v>
+      </c>
+      <c r="AD35">
+        <v>7.3625520278701604</v>
+      </c>
+      <c r="AE35">
+        <v>6.5774706409666299</v>
+      </c>
+      <c r="AF35">
+        <v>6.4450756904956403</v>
+      </c>
+      <c r="AG35">
+        <v>8.9165148387612607</v>
+      </c>
+      <c r="AJ35" s="2">
+        <f t="shared" si="2"/>
+        <v>8.7698047774647314</v>
+      </c>
+      <c r="AK35" s="2">
+        <f t="shared" si="3"/>
+        <v>1.8616527422573153</v>
+      </c>
+      <c r="AL35">
+        <v>8.7698047774647314</v>
+      </c>
+    </row>
+    <row r="36" spans="4:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AF36" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI36" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ36" s="2"/>
+      <c r="AK36" s="2"/>
+    </row>
+    <row r="37" spans="4:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AF37" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI37" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK37" s="2"/>
+    </row>
+    <row r="38" spans="4:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>6.8759087028996904</v>
+      </c>
+      <c r="E38">
+        <v>7.51523641696767</v>
+      </c>
+      <c r="F38">
+        <v>5.6918993332357601</v>
+      </c>
+      <c r="G38">
+        <v>5.4496817476921002</v>
+      </c>
+      <c r="H38">
+        <v>4.4371479466992501</v>
+      </c>
+      <c r="I38">
+        <v>6.4544977077942196</v>
+      </c>
+      <c r="J38">
+        <v>6.7169615328972903</v>
+      </c>
+      <c r="K38">
+        <v>8.3030862194037809</v>
+      </c>
+      <c r="L38">
+        <v>5.0936090394835203</v>
+      </c>
+      <c r="M38">
+        <v>5.2842553989032801</v>
+      </c>
+      <c r="N38">
+        <v>8.0544786477688994</v>
+      </c>
+      <c r="O38">
+        <v>4.5074918166385904</v>
+      </c>
+      <c r="P38">
+        <v>7.2231424477243404</v>
+      </c>
+      <c r="Q38">
+        <v>7.1039640247616003</v>
+      </c>
+      <c r="R38">
+        <v>7.0041485874446696</v>
+      </c>
+      <c r="S38">
+        <v>5.7905539841693701</v>
+      </c>
+      <c r="T38">
+        <v>5.84634731242586</v>
+      </c>
+      <c r="U38">
+        <v>6.0087364741299796</v>
+      </c>
+      <c r="V38">
+        <v>9.3441523052150899</v>
+      </c>
+      <c r="W38">
+        <v>5.0910434072631503</v>
+      </c>
+      <c r="X38">
+        <v>5.86214192470936</v>
+      </c>
+      <c r="Y38">
+        <v>4.1506389500563801</v>
+      </c>
+      <c r="Z38">
+        <v>4.6605346826536804</v>
+      </c>
+      <c r="AA38">
+        <v>7.2973115957009496</v>
+      </c>
+      <c r="AB38">
+        <v>8.5292095236525505</v>
+      </c>
+      <c r="AC38">
+        <v>2.9827916387631399</v>
+      </c>
+      <c r="AD38">
+        <v>6.2622778380322002</v>
+      </c>
+      <c r="AE38">
+        <v>5.6872760268770497</v>
+      </c>
+      <c r="AF38">
+        <v>7.6436065289407704</v>
+      </c>
+      <c r="AG38">
+        <v>4.3021631951043702</v>
+      </c>
+      <c r="AJ38" s="2">
+        <f t="shared" ref="AJ38:AL41" si="4">AVERAGE(D38:AG38)</f>
+        <v>6.1724764986002869</v>
+      </c>
+      <c r="AK38" s="2">
+        <f t="shared" ref="AK38:AK41" si="5">_xlfn.STDEV.S(D38:AG38)</f>
+        <v>1.4714031720181491</v>
+      </c>
+      <c r="AL38">
+        <v>6.1724764986002869</v>
+      </c>
+    </row>
+    <row r="39" spans="4:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>8.2634265285434392</v>
+      </c>
+      <c r="E39">
+        <v>13.7673062594661</v>
+      </c>
+      <c r="F39">
+        <v>14.7622959818396</v>
+      </c>
+      <c r="G39">
+        <v>7.1231116773380396</v>
+      </c>
+      <c r="H39">
+        <v>6.2365541166643697</v>
+      </c>
+      <c r="I39">
+        <v>5.6673260755943202</v>
+      </c>
+      <c r="J39">
+        <v>10.6642067920366</v>
+      </c>
+      <c r="K39">
+        <v>5.1033854989835499</v>
+      </c>
+      <c r="L39">
+        <v>10.541798452145001</v>
+      </c>
+      <c r="M39">
+        <v>12.8195107927799</v>
+      </c>
+      <c r="N39">
+        <v>6.00302060889</v>
+      </c>
+      <c r="O39">
+        <v>12.488082339936501</v>
+      </c>
+      <c r="P39">
+        <v>7.9933813436691104</v>
+      </c>
+      <c r="Q39">
+        <v>8.8162817009592391</v>
+      </c>
+      <c r="R39">
+        <v>12.0580254578959</v>
+      </c>
+      <c r="S39">
+        <v>10.030862770724999</v>
+      </c>
+      <c r="T39">
+        <v>7.4797093344042898</v>
+      </c>
+      <c r="U39">
+        <v>9.9653163856369709</v>
+      </c>
+      <c r="V39">
+        <v>11.737356847764699</v>
+      </c>
+      <c r="W39">
+        <v>8.9914159874948396</v>
+      </c>
+      <c r="X39">
+        <v>7.9166909808493102</v>
+      </c>
+      <c r="Y39">
+        <v>7.5242056371794002</v>
+      </c>
+      <c r="Z39">
+        <v>12.8150898714494</v>
+      </c>
+      <c r="AA39">
+        <v>8.2702213929642703</v>
+      </c>
+      <c r="AB39">
+        <v>6.4842366702130603</v>
+      </c>
+      <c r="AC39">
+        <v>10.4575099816098</v>
+      </c>
+      <c r="AD39">
+        <v>10.604741802661801</v>
+      </c>
+      <c r="AE39">
+        <v>12.8943816810567</v>
+      </c>
+      <c r="AF39">
+        <v>9.9271366350223094</v>
+      </c>
+      <c r="AG39">
+        <v>6.6026196861036803</v>
+      </c>
+      <c r="AJ39" s="2">
+        <f t="shared" si="4"/>
+        <v>9.4669736430625715</v>
+      </c>
+      <c r="AK39" s="2">
+        <f t="shared" si="5"/>
+        <v>2.6372916568441616</v>
+      </c>
+      <c r="AL39">
+        <v>9.4669736430625715</v>
+      </c>
+    </row>
+    <row r="40" spans="4:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>5.7947940394433504</v>
+      </c>
+      <c r="E40">
+        <v>10.7362678485394</v>
+      </c>
+      <c r="F40">
+        <v>15.9890388185287</v>
+      </c>
+      <c r="G40">
+        <v>7.0070331358614002</v>
+      </c>
+      <c r="H40">
+        <v>9.5148299771696898</v>
+      </c>
+      <c r="I40">
+        <v>9.5431157235212005</v>
+      </c>
+      <c r="J40">
+        <v>10.918049808670199</v>
+      </c>
+      <c r="K40">
+        <v>9.1705179098295595</v>
+      </c>
+      <c r="L40">
+        <v>6.6150235163130304</v>
+      </c>
+      <c r="M40">
+        <v>7.7548823531556099</v>
+      </c>
+      <c r="N40">
+        <v>8.2229215167410601</v>
+      </c>
+      <c r="O40">
+        <v>7.5272578999608397</v>
+      </c>
+      <c r="P40">
+        <v>13.212412578106401</v>
+      </c>
+      <c r="Q40">
+        <v>13.702278352327999</v>
+      </c>
+      <c r="R40">
+        <v>11.1050672405866</v>
+      </c>
+      <c r="S40">
+        <v>6.1208463168943599</v>
+      </c>
+      <c r="T40">
+        <v>8.2476135035448408</v>
+      </c>
+      <c r="U40">
+        <v>8.5140046449457998</v>
+      </c>
+      <c r="V40">
+        <v>7.7258254026833102</v>
+      </c>
+      <c r="W40">
+        <v>7.6798068347465902</v>
+      </c>
+      <c r="X40">
+        <v>10.4637782450815</v>
+      </c>
+      <c r="Y40">
+        <v>3.9923920680604801</v>
+      </c>
+      <c r="Z40">
+        <v>12.3305322091185</v>
+      </c>
+      <c r="AA40">
+        <v>10.637098547534301</v>
+      </c>
+      <c r="AB40">
+        <v>6.8540567739464597</v>
+      </c>
+      <c r="AC40">
+        <v>9.8454771882772807</v>
+      </c>
+      <c r="AD40">
+        <v>14.483280899083001</v>
+      </c>
+      <c r="AE40">
+        <v>21.550252754954801</v>
+      </c>
+      <c r="AF40" s="4">
+        <v>6.9141102586989804</v>
+      </c>
+      <c r="AG40">
+        <v>7.9142106273434303</v>
+      </c>
+      <c r="AJ40" s="2">
+        <f t="shared" si="4"/>
+        <v>9.6695592331222908</v>
+      </c>
+      <c r="AK40" s="2">
+        <f t="shared" si="5"/>
+        <v>3.5384500199676752</v>
+      </c>
+      <c r="AL40">
+        <v>9.6695592331222908</v>
+      </c>
+    </row>
+    <row r="41" spans="4:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>14.354413130432</v>
+      </c>
+      <c r="E41">
+        <v>10.695212401973899</v>
+      </c>
+      <c r="F41">
+        <v>7.5937402171454904</v>
+      </c>
+      <c r="G41">
+        <v>9.1872774616864703</v>
+      </c>
+      <c r="H41">
+        <v>9.4023633719500292</v>
+      </c>
+      <c r="I41">
+        <v>7.6088923356291698</v>
+      </c>
+      <c r="J41">
+        <v>17.8185688099713</v>
+      </c>
+      <c r="K41">
+        <v>22.104206492233001</v>
+      </c>
+      <c r="L41">
+        <v>5.9352393010558204</v>
+      </c>
+      <c r="M41">
+        <v>13.4683167447036</v>
+      </c>
+      <c r="N41">
+        <v>6.7035190900857904</v>
+      </c>
+      <c r="O41">
+        <v>9.2309639167441109</v>
+      </c>
+      <c r="P41">
+        <v>8.3215057160104493</v>
+      </c>
+      <c r="Q41">
+        <v>12.309987079739599</v>
+      </c>
+      <c r="R41">
+        <v>7.8568257281139999</v>
+      </c>
+      <c r="S41">
+        <v>13.506959652023999</v>
+      </c>
+      <c r="T41">
+        <v>9.7734920956794706</v>
+      </c>
+      <c r="U41">
+        <v>12.036346836156399</v>
+      </c>
+      <c r="V41">
+        <v>4.4724552292030699</v>
+      </c>
+      <c r="W41">
+        <v>11.0177964845284</v>
+      </c>
+      <c r="X41">
+        <v>11.2958675274597</v>
+      </c>
+      <c r="Y41">
+        <v>10.580847620240901</v>
+      </c>
+      <c r="Z41">
+        <v>10.7460277760491</v>
+      </c>
+      <c r="AA41">
+        <v>6.0781952613401202</v>
+      </c>
+      <c r="AB41">
+        <v>16.1503733820307</v>
+      </c>
+      <c r="AC41">
+        <v>13.6220620179162</v>
+      </c>
+      <c r="AD41">
+        <v>9.8077600223441106</v>
+      </c>
+      <c r="AE41">
+        <v>16.6317718803143</v>
+      </c>
+      <c r="AF41">
+        <v>9.9846441788084306</v>
+      </c>
+      <c r="AG41">
+        <v>25.439684976621098</v>
+      </c>
+      <c r="AJ41" s="2">
+        <f t="shared" si="4"/>
+        <v>11.457843891273024</v>
+      </c>
+      <c r="AK41" s="2">
+        <f t="shared" si="5"/>
+        <v>4.6534983170888626</v>
+      </c>
+      <c r="AL41">
+        <v>11.457843891273024</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Estable, estoy a punto de cambiar los nombre de los archivos de simulación
</commit_message>
<xml_diff>
--- a/Proyecto/Caso5.xlsx
+++ b/Proyecto/Caso5.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="9975" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="9975" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="1 cluster" sheetId="4" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="34">
   <si>
     <t>Clusters 1</t>
   </si>
@@ -105,6 +105,18 @@
   </si>
   <si>
     <t>dipolo</t>
+  </si>
+  <si>
+    <t>caso 1</t>
+  </si>
+  <si>
+    <t>caso 2</t>
+  </si>
+  <si>
+    <t>caso 3</t>
+  </si>
+  <si>
+    <t>caso 4</t>
   </si>
 </sst>
 </file>
@@ -469,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:BL91"/>
   <sheetViews>
-    <sheetView topLeftCell="AT1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AV9" sqref="AV9"/>
+    <sheetView tabSelected="1" topLeftCell="AD12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AJ16" sqref="AJ16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,6 +692,9 @@
       <c r="AG8">
         <v>4.82927704132186</v>
       </c>
+      <c r="AI8" t="s">
+        <v>30</v>
+      </c>
       <c r="AJ8" s="2">
         <f>AVERAGE(D8:AG8)</f>
         <v>4.3151562145125215</v>
@@ -703,11 +718,11 @@
         <v>4.1030539582227208</v>
       </c>
       <c r="AX8" s="6">
-        <f>AV8-AW8</f>
+        <f t="shared" ref="AX8:AX13" si="0">AV8-AW8</f>
         <v>0.21210225628980073</v>
       </c>
       <c r="AY8" s="6">
-        <f>(AV8/AW8-1)*100</f>
+        <f t="shared" ref="AY8:AY13" si="1">(AV8/AW8-1)*100</f>
         <v>5.1693752616813082</v>
       </c>
       <c r="BE8">
@@ -813,6 +828,9 @@
       </c>
       <c r="AG9">
         <v>4.2314388398934097</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>32</v>
       </c>
       <c r="AJ9" s="2">
         <f>AVERAGE(D9:AG9)</f>
@@ -837,11 +855,11 @@
         <v>4.2217867287734689</v>
       </c>
       <c r="AX9" s="6">
-        <f>AV9-AW9</f>
+        <f t="shared" si="0"/>
         <v>0.43890499145619266</v>
       </c>
       <c r="AY9" s="6">
-        <f>(AV9/AW9-1)*100</f>
+        <f t="shared" si="1"/>
         <v>10.396190514903282</v>
       </c>
       <c r="BE9">
@@ -951,12 +969,15 @@
       <c r="AG10">
         <v>4.9505648588313003</v>
       </c>
+      <c r="AI10" t="s">
+        <v>31</v>
+      </c>
       <c r="AJ10" s="2">
-        <f t="shared" ref="AJ10:AJ17" si="0">AVERAGE(D10:AG10)</f>
+        <f t="shared" ref="AJ10:AJ17" si="2">AVERAGE(D10:AG10)</f>
         <v>4.7437911226340193</v>
       </c>
       <c r="AK10" s="2">
-        <f t="shared" ref="AK10:AK17" si="1">_xlfn.STDEV.S(D10:AG10)</f>
+        <f t="shared" ref="AK10:AK17" si="3">_xlfn.STDEV.S(D10:AG10)</f>
         <v>0.27914644619304174</v>
       </c>
       <c r="AM10" s="2"/>
@@ -974,23 +995,23 @@
         <v>6.5052084755275654</v>
       </c>
       <c r="AX10" s="6">
-        <f>AV10-AW10</f>
+        <f t="shared" si="0"/>
         <v>0.58562305494649891</v>
       </c>
       <c r="AY10" s="6">
-        <f>(AV10/AW10-1)*100</f>
+        <f t="shared" si="1"/>
         <v>9.002371824816958</v>
       </c>
       <c r="BE10">
-        <f t="shared" ref="BE10:BI10" si="2">BE8-BE9</f>
+        <f t="shared" ref="BE10:BI10" si="4">BE8-BE9</f>
         <v>-0.14347946375959886</v>
       </c>
       <c r="BG10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.54708934769513551</v>
       </c>
       <c r="BI10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-0.2771232257303291</v>
       </c>
       <c r="BJ10" t="s">
@@ -1094,12 +1115,15 @@
       <c r="AG11">
         <v>4.08878568812883</v>
       </c>
+      <c r="AI11" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.2568917664147978</v>
       </c>
       <c r="AK11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.41821584522787525</v>
       </c>
       <c r="AM11" s="2"/>
@@ -1117,23 +1141,23 @@
         <v>6.6160894971757473</v>
       </c>
       <c r="AX11" s="6">
-        <f>AV11-AW11</f>
+        <f t="shared" si="0"/>
         <v>1.4013790946647982</v>
       </c>
       <c r="AY11" s="6">
-        <f>(AV11/AW11-1)*100</f>
+        <f t="shared" si="1"/>
         <v>21.181380561176113</v>
       </c>
       <c r="BE11">
-        <f t="shared" ref="BE11:BI11" si="3">(BE8/BE9-1)*100</f>
+        <f t="shared" ref="BE11:BI11" si="5">(BE8/BE9-1)*100</f>
         <v>-3.2184509023987173</v>
       </c>
       <c r="BG11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>13.036174048919701</v>
       </c>
       <c r="BI11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-6.1120932817916636</v>
       </c>
       <c r="BJ11" t="s">
@@ -1170,11 +1194,11 @@
         <v>8.5196521018960976</v>
       </c>
       <c r="AX12" s="6">
-        <f>AV12-AW12</f>
+        <f t="shared" si="0"/>
         <v>0.82202931851819372</v>
       </c>
       <c r="AY12" s="6">
-        <f>(AV12/AW12-1)*100</f>
+        <f t="shared" si="1"/>
         <v>9.6486254213977496</v>
       </c>
       <c r="BJ12" t="s">
@@ -1220,11 +1244,11 @@
         <v>8.4025380938040506</v>
       </c>
       <c r="AX13" s="6">
-        <f>AV13-AW13</f>
+        <f t="shared" si="0"/>
         <v>3.7835796235971539</v>
       </c>
       <c r="AY13" s="6">
-        <f>(AV13/AW13-1)*100</f>
+        <f t="shared" si="1"/>
         <v>45.029008870392715</v>
       </c>
       <c r="BE13" t="s">
@@ -1328,12 +1352,15 @@
       <c r="AG14">
         <v>4.7349386360690904</v>
       </c>
+      <c r="AI14" t="s">
+        <v>30</v>
+      </c>
       <c r="AJ14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.6606917202296616</v>
       </c>
       <c r="AK14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.31818483061429803</v>
       </c>
       <c r="AL14" s="5">
@@ -1460,12 +1487,15 @@
       <c r="AG15">
         <v>3.7829795368213999</v>
       </c>
+      <c r="AI15" t="s">
+        <v>32</v>
+      </c>
       <c r="AJ15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.3902911864138776</v>
       </c>
       <c r="AK15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.38226562226030902</v>
       </c>
       <c r="AM15" s="1"/>
@@ -1580,12 +1610,15 @@
       <c r="AG16">
         <v>7.3156162144291104</v>
       </c>
+      <c r="AI16" t="s">
+        <v>31</v>
+      </c>
       <c r="AJ16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.9005155587113736</v>
       </c>
       <c r="AK16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.6944246390510167</v>
       </c>
       <c r="AM16" s="1"/>
@@ -1594,15 +1627,15 @@
       <c r="AP16" s="1"/>
       <c r="AQ16" s="1"/>
       <c r="BE16">
-        <f t="shared" ref="BE16" si="4">BE14-BE15</f>
+        <f t="shared" ref="BE16" si="6">BE14-BE15</f>
         <v>-4.2934851283323638E-2</v>
       </c>
       <c r="BG16">
-        <f t="shared" ref="BG16" si="5">BG14-BG15</f>
+        <f t="shared" ref="BG16" si="7">BG14-BG15</f>
         <v>2.5795684075785248</v>
       </c>
       <c r="BI16">
-        <f t="shared" ref="BI16" si="6">BI14-BI15</f>
+        <f t="shared" ref="BI16" si="8">BI14-BI15</f>
         <v>1.2764022491732874</v>
       </c>
       <c r="BJ16" t="s">
@@ -1706,12 +1739,15 @@
       <c r="AG17">
         <v>10.0695333217765</v>
       </c>
+      <c r="AI17" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.7969225427667022</v>
       </c>
       <c r="AK17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.9195844794495021</v>
       </c>
       <c r="AM17" s="1"/>
@@ -1735,15 +1771,15 @@
         <v>18</v>
       </c>
       <c r="BE17">
-        <f t="shared" ref="BE17:BI17" si="7">(BE14/BE15-1)*100</f>
+        <f t="shared" ref="BE17:BI17" si="9">(BE14/BE15-1)*100</f>
         <v>-0.96847873124975559</v>
       </c>
       <c r="BG17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>59.699142742401378</v>
       </c>
       <c r="BI17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>28.235737620340593</v>
       </c>
       <c r="BJ17" t="s">
@@ -1783,11 +1819,11 @@
         <v>4.1967017749388837</v>
       </c>
       <c r="AZ18" s="5">
-        <f>AX18-AY18</f>
+        <f t="shared" ref="AZ18:AZ23" si="10">AX18-AY18</f>
         <v>0.54708934769513551</v>
       </c>
       <c r="BA18" s="5">
-        <f>(AX18/AY18-1)*100</f>
+        <f t="shared" ref="BA18:BA23" si="11">(AX18/AY18-1)*100</f>
         <v>13.036174048919701</v>
       </c>
       <c r="BJ18" t="s">
@@ -1839,11 +1875,11 @@
         <v>4.3209471511328488</v>
       </c>
       <c r="AZ19" s="5">
-        <f>AX19-AY19</f>
+        <f t="shared" si="10"/>
         <v>2.5795684075785248</v>
       </c>
       <c r="BA19" s="5">
-        <f>(AX19/AY19-1)*100</f>
+        <f t="shared" si="11"/>
         <v>59.699142742401378</v>
       </c>
       <c r="BE19" t="s">
@@ -1947,12 +1983,15 @@
       <c r="AG20">
         <v>7.7585501244283801</v>
       </c>
+      <c r="AI20" t="s">
+        <v>30</v>
+      </c>
       <c r="AJ20" s="2">
-        <f t="shared" ref="AJ20:AJ35" si="8">AVERAGE(D20:AG20)</f>
+        <f t="shared" ref="AJ20:AJ35" si="12">AVERAGE(D20:AG20)</f>
         <v>7.0908315304740643</v>
       </c>
       <c r="AK20" s="2">
-        <f t="shared" ref="AK20:AK35" si="9">_xlfn.STDEV.S(D20:AG20)</f>
+        <f t="shared" ref="AK20:AK35" si="13">_xlfn.STDEV.S(D20:AG20)</f>
         <v>0.59932276661002337</v>
       </c>
       <c r="AL20" s="5">
@@ -1983,11 +2022,11 @@
         <v>6.9237412333723753</v>
       </c>
       <c r="AZ20" s="5">
-        <f>AX20-AY20</f>
+        <f t="shared" si="10"/>
         <v>1.1488837989828031</v>
       </c>
       <c r="BA20" s="5">
-        <f>(AX20/AY20-1)*100</f>
+        <f t="shared" si="11"/>
         <v>16.593395972760973</v>
       </c>
       <c r="BE20">
@@ -2094,12 +2133,15 @@
       <c r="AG21">
         <v>13.294411021811101</v>
       </c>
+      <c r="AI21" t="s">
+        <v>32</v>
+      </c>
       <c r="AJ21" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>8.5893338627309852</v>
       </c>
       <c r="AK21" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1.7083251276102449</v>
       </c>
       <c r="AL21" s="5"/>
@@ -2118,11 +2160,11 @@
         <v>7.2199455498044021</v>
       </c>
       <c r="AZ21" s="5">
-        <f>AX21-AY21</f>
+        <f t="shared" si="10"/>
         <v>5.5314140270854679</v>
       </c>
       <c r="BA21" s="5">
-        <f>(AX21/AY21-1)*100</f>
+        <f t="shared" si="11"/>
         <v>76.612960429255892</v>
       </c>
       <c r="BE21">
@@ -2232,12 +2274,15 @@
       <c r="AG22">
         <v>8.2471558472062299</v>
       </c>
+      <c r="AI22" t="s">
+        <v>31</v>
+      </c>
       <c r="AJ22" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>8.0726250323551785</v>
       </c>
       <c r="AK22" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0.52762908601412395</v>
       </c>
       <c r="AL22" s="5"/>
@@ -2256,23 +2301,23 @@
         <v>10.559459629389412</v>
       </c>
       <c r="AZ22" s="5">
-        <f>AX22-AY22</f>
+        <f t="shared" si="10"/>
         <v>2.104610959087605</v>
       </c>
       <c r="BA22" s="5">
-        <f>(AX22/AY22-1)*100</f>
+        <f t="shared" si="11"/>
         <v>19.931047922471222</v>
       </c>
       <c r="BE22">
-        <f t="shared" ref="BE22" si="10">BE20-BE21</f>
+        <f t="shared" ref="BE22" si="14">BE20-BE21</f>
         <v>-1.048930895920364</v>
       </c>
       <c r="BG22">
-        <f t="shared" ref="BG22" si="11">BG20-BG21</f>
+        <f t="shared" ref="BG22" si="15">BG20-BG21</f>
         <v>1.1488837989828031</v>
       </c>
       <c r="BI22">
-        <f t="shared" ref="BI22" si="12">BI20-BI21</f>
+        <f t="shared" ref="BI22" si="16">BI20-BI21</f>
         <v>-0.69253716958921707</v>
       </c>
       <c r="BJ22" t="s">
@@ -2376,12 +2421,15 @@
       <c r="AG23">
         <v>6.9410372941723999</v>
       </c>
+      <c r="AI23" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ23" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>9.4339768321203703</v>
       </c>
       <c r="AK23" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1.1512915599638371</v>
       </c>
       <c r="AL23" s="5"/>
@@ -2403,23 +2451,23 @@
         <v>10.774963435890092</v>
       </c>
       <c r="AZ23" s="5">
-        <f>AX23-AY23</f>
+        <f t="shared" si="10"/>
         <v>12.605602240214358</v>
       </c>
       <c r="BA23" s="5">
-        <f>(AX23/AY23-1)*100</f>
+        <f t="shared" si="11"/>
         <v>116.98974493246661</v>
       </c>
       <c r="BE23">
-        <f t="shared" ref="BE23:BI23" si="13">(BE20/BE21-1)*100</f>
+        <f t="shared" ref="BE23:BI23" si="17">(BE20/BE21-1)*100</f>
         <v>-10.882984875247793</v>
       </c>
       <c r="BG23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>16.593395972760973</v>
       </c>
       <c r="BI23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>-6.8388506594895482</v>
       </c>
       <c r="BJ23" t="s">
@@ -2590,12 +2638,15 @@
       <c r="AG26">
         <v>7.9620834761209904</v>
       </c>
+      <c r="AI26" t="s">
+        <v>30</v>
+      </c>
       <c r="AJ26" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>8.0174685918405455</v>
       </c>
       <c r="AK26" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0.63282827944364273</v>
       </c>
       <c r="AL26" s="5">
@@ -2717,12 +2768,15 @@
       <c r="AG27">
         <v>6.7048149299311204</v>
       </c>
+      <c r="AI27" t="s">
+        <v>32</v>
+      </c>
       <c r="AJ27" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>8.6190510001893657</v>
       </c>
       <c r="AK27" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1.3132287730918499</v>
       </c>
       <c r="AL27" s="5"/>
@@ -2844,12 +2898,15 @@
       <c r="AG28">
         <v>20.775179319248</v>
       </c>
+      <c r="AI28" t="s">
+        <v>31</v>
+      </c>
       <c r="AJ28" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>12.75135957688987</v>
       </c>
       <c r="AK28" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>2.8940643511753077</v>
       </c>
       <c r="AL28" s="5"/>
@@ -2868,23 +2925,23 @@
         <v>4.4580286638103868</v>
       </c>
       <c r="AZ28" s="5">
-        <f>AX28-AY28</f>
+        <f t="shared" ref="AZ28:AZ33" si="18">AX28-AY28</f>
         <v>-0.14347946375959886</v>
       </c>
       <c r="BA28" s="5">
-        <f>(AX28/AY28-1)*100</f>
+        <f t="shared" ref="BA28:BA33" si="19">(AX28/AY28-1)*100</f>
         <v>-3.2184509023987173</v>
       </c>
       <c r="BE28">
-        <f t="shared" ref="BE28" si="14">BE26-BE27</f>
+        <f t="shared" ref="BE28" si="20">BE26-BE27</f>
         <v>-1.1827886752354377</v>
       </c>
       <c r="BG28">
-        <f t="shared" ref="BG28" si="15">BG26-BG27</f>
+        <f t="shared" ref="BG28" si="21">BG26-BG27</f>
         <v>5.5314140270854679</v>
       </c>
       <c r="BI28">
-        <f t="shared" ref="BI28" si="16">BI26-BI27</f>
+        <f t="shared" ref="BI28" si="22">BI26-BI27</f>
         <v>0.83884807332186995</v>
       </c>
     </row>
@@ -2979,12 +3036,15 @@
       <c r="AG29">
         <v>9.9048778563608799</v>
       </c>
+      <c r="AI29" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ29" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>10.902809543502425</v>
       </c>
       <c r="AK29" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>3.0652320075246342</v>
       </c>
       <c r="AL29" s="5"/>
@@ -3006,23 +3066,23 @@
         <v>4.4332260376972012</v>
       </c>
       <c r="AZ29" s="5">
-        <f>AX29-AY29</f>
+        <f t="shared" si="18"/>
         <v>-4.2934851283323638E-2</v>
       </c>
       <c r="BA29" s="5">
-        <f>(AX29/AY29-1)*100</f>
+        <f t="shared" si="19"/>
         <v>-0.96847873124975559</v>
       </c>
       <c r="BE29">
-        <f t="shared" ref="BE29:BI29" si="17">(BE26/BE27-1)*100</f>
+        <f t="shared" ref="BE29:BI29" si="23">(BE26/BE27-1)*100</f>
         <v>-12.067006953816318</v>
       </c>
       <c r="BG29">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>76.612960429255892</v>
       </c>
       <c r="BI29">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>8.3351677747114827</v>
       </c>
     </row>
@@ -3054,11 +3114,11 @@
         <v>9.6382647586513492</v>
       </c>
       <c r="AZ30" s="5">
-        <f>AX30-AY30</f>
+        <f t="shared" si="18"/>
         <v>-1.048930895920364</v>
       </c>
       <c r="BA30" s="5">
-        <f>(AX30/AY30-1)*100</f>
+        <f t="shared" si="19"/>
         <v>-10.882984875247793</v>
       </c>
     </row>
@@ -3101,11 +3161,11 @@
         <v>9.8018396754248034</v>
       </c>
       <c r="AZ31" s="5">
-        <f>AX31-AY31</f>
+        <f t="shared" si="18"/>
         <v>-1.1827886752354377</v>
       </c>
       <c r="BA31" s="5">
-        <f>(AX31/AY31-1)*100</f>
+        <f t="shared" si="19"/>
         <v>-12.067006953816318</v>
       </c>
       <c r="BE31" t="s">
@@ -3209,12 +3269,15 @@
       <c r="AG32">
         <v>8.9292585727315803</v>
       </c>
+      <c r="AI32" t="s">
+        <v>30</v>
+      </c>
       <c r="AJ32" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>9.3416814204142913</v>
       </c>
       <c r="AK32" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1.110498757620775</v>
       </c>
       <c r="AL32" s="5">
@@ -3245,11 +3308,11 @@
         <v>16.216907711420916</v>
       </c>
       <c r="AZ32" s="5">
-        <f>AX32-AY32</f>
+        <f t="shared" si="18"/>
         <v>-0.84250456220830117</v>
       </c>
       <c r="BA32" s="5">
-        <f>(AX32/AY32-1)*100</f>
+        <f t="shared" si="19"/>
         <v>-5.1952232645127499</v>
       </c>
       <c r="BE32">
@@ -3353,12 +3416,15 @@
       <c r="AG33">
         <v>15.7100907331368</v>
       </c>
+      <c r="AI33" t="s">
+        <v>32</v>
+      </c>
       <c r="AJ33" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>15.374403149212615</v>
       </c>
       <c r="AK33" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>2.5991176303019512</v>
       </c>
       <c r="AL33" s="5"/>
@@ -3377,11 +3443,11 @@
         <v>15.944082701894363</v>
       </c>
       <c r="AZ33" s="5">
-        <f>AX33-AY33</f>
+        <f t="shared" si="18"/>
         <v>1.0434303104461442</v>
       </c>
       <c r="BA33" s="5">
-        <f>(AX33/AY33-1)*100</f>
+        <f t="shared" si="19"/>
         <v>6.5443107010613399</v>
       </c>
       <c r="BE33">
@@ -3485,12 +3551,15 @@
       <c r="AG34">
         <v>12.7889528948216</v>
       </c>
+      <c r="AI34" t="s">
+        <v>31</v>
+      </c>
       <c r="AJ34" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>12.664070588477017</v>
       </c>
       <c r="AK34" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1.1907723989377514</v>
       </c>
       <c r="AL34" s="5"/>
@@ -3500,15 +3569,15 @@
       <c r="AP34" s="2"/>
       <c r="AQ34" s="2"/>
       <c r="BE34">
-        <f t="shared" ref="BE34" si="18">BE32-BE33</f>
+        <f t="shared" ref="BE34" si="24">BE32-BE33</f>
         <v>-0.84250456220830117</v>
       </c>
       <c r="BG34">
-        <f t="shared" ref="BG34" si="19">BG32-BG33</f>
+        <f t="shared" ref="BG34" si="25">BG32-BG33</f>
         <v>2.104610959087605</v>
       </c>
       <c r="BI34">
-        <f t="shared" ref="BI34" si="20">BI32-BI33</f>
+        <f t="shared" ref="BI34" si="26">BI32-BI33</f>
         <v>-0.39356564809921579</v>
       </c>
     </row>
@@ -3603,12 +3672,15 @@
       <c r="AG35">
         <v>22.189920552475201</v>
       </c>
+      <c r="AI35" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ35" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>18.711215843700355</v>
       </c>
       <c r="AK35" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>2.7167443958416784</v>
       </c>
       <c r="AL35" s="5"/>
@@ -3621,15 +3693,15 @@
         <v>18</v>
       </c>
       <c r="BE35">
-        <f t="shared" ref="BE35:BI35" si="21">(BE32/BE33-1)*100</f>
+        <f t="shared" ref="BE35:BI35" si="27">(BE32/BE33-1)*100</f>
         <v>-5.1952232645127499</v>
       </c>
       <c r="BG35">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>19.931047922471222</v>
       </c>
       <c r="BI35">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>-2.0600374218786466</v>
       </c>
     </row>
@@ -3703,11 +3775,11 @@
         <v>4.5340149921451269</v>
       </c>
       <c r="AZ37" s="5">
-        <f>AX37-AY37</f>
+        <f t="shared" ref="AZ37:AZ42" si="28">AX37-AY37</f>
         <v>-0.2771232257303291</v>
       </c>
       <c r="BA37" s="5">
-        <f>(AX37/AY37-1)*100</f>
+        <f t="shared" ref="BA37:BA42" si="29">(AX37/AY37-1)*100</f>
         <v>-6.1120932817916636</v>
       </c>
       <c r="BE37" t="s">
@@ -3811,12 +3883,15 @@
       <c r="AG38">
         <v>12.708205534623</v>
       </c>
+      <c r="AI38" t="s">
+        <v>30</v>
+      </c>
       <c r="AJ38" s="2">
-        <f t="shared" ref="AJ38:AJ41" si="22">AVERAGE(D38:AG38)</f>
+        <f t="shared" ref="AJ38:AJ41" si="30">AVERAGE(D38:AG38)</f>
         <v>12.186117717401205</v>
       </c>
       <c r="AK38" s="2">
-        <f t="shared" ref="AK38:AK41" si="23">_xlfn.STDEV.S(D38:AG38)</f>
+        <f t="shared" ref="AK38:AK41" si="31">_xlfn.STDEV.S(D38:AG38)</f>
         <v>1.5543448361996259</v>
       </c>
       <c r="AL38" s="2">
@@ -3847,11 +3922,11 @@
         <v>4.5205202935934148</v>
       </c>
       <c r="AZ38" s="5">
-        <f>AX38-AY38</f>
+        <f t="shared" si="28"/>
         <v>1.2764022491732874</v>
       </c>
       <c r="BA38" s="5">
-        <f>(AX38/AY38-1)*100</f>
+        <f t="shared" si="29"/>
         <v>28.235737620340593</v>
       </c>
       <c r="BE38">
@@ -3955,12 +4030,15 @@
       <c r="AG39">
         <v>12.0706517018996</v>
       </c>
+      <c r="AI39" t="s">
+        <v>32</v>
+      </c>
       <c r="AJ39" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>16.987513012340507</v>
       </c>
       <c r="AK39" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="31"/>
         <v>3.8142685872044444</v>
       </c>
       <c r="AM39" s="2"/>
@@ -3978,11 +4056,11 @@
         <v>10.126514001709587</v>
       </c>
       <c r="AZ39" s="5">
-        <f>AX39-AY39</f>
+        <f t="shared" si="28"/>
         <v>-0.69253716958921707</v>
       </c>
       <c r="BA39" s="5">
-        <f>(AX39/AY39-1)*100</f>
+        <f t="shared" si="29"/>
         <v>-6.8388506594895482</v>
       </c>
       <c r="BE39">
@@ -4086,12 +4164,15 @@
       <c r="AG40">
         <v>33.075049130053699</v>
       </c>
+      <c r="AI40" t="s">
+        <v>31</v>
+      </c>
       <c r="AJ40" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>23.38056567610445</v>
       </c>
       <c r="AK40" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="31"/>
         <v>5.4029592432716465</v>
       </c>
       <c r="AM40" s="2"/>
@@ -4109,23 +4190,23 @@
         <v>10.063961470180555</v>
       </c>
       <c r="AZ40" s="5">
-        <f>AX40-AY40</f>
+        <f t="shared" si="28"/>
         <v>0.83884807332186995</v>
       </c>
       <c r="BA40" s="5">
-        <f>(AX40/AY40-1)*100</f>
+        <f t="shared" si="29"/>
         <v>8.3351677747114827</v>
       </c>
       <c r="BE40">
-        <f t="shared" ref="BE40" si="24">BE38-BE39</f>
+        <f t="shared" ref="BE40" si="32">BE38-BE39</f>
         <v>1.0434303104461442</v>
       </c>
       <c r="BG40">
-        <f t="shared" ref="BG40" si="25">BG38-BG39</f>
+        <f t="shared" ref="BG40" si="33">BG38-BG39</f>
         <v>12.605602240214358</v>
       </c>
       <c r="BI40">
-        <f t="shared" ref="BI40" si="26">BI38-BI39</f>
+        <f t="shared" ref="BI40" si="34">BI38-BI39</f>
         <v>10.424598217110233</v>
       </c>
     </row>
@@ -4220,12 +4301,15 @@
       <c r="AG41">
         <v>52.991459776885399</v>
       </c>
+      <c r="AI41" t="s">
+        <v>33</v>
+      </c>
       <c r="AJ41" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>29.32912838340696</v>
       </c>
       <c r="AK41" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="31"/>
         <v>11.021409584412559</v>
       </c>
       <c r="AM41" s="2"/>
@@ -4246,23 +4330,23 @@
         <v>19.104781491799571</v>
       </c>
       <c r="AZ41" s="5">
-        <f>AX41-AY41</f>
+        <f t="shared" si="28"/>
         <v>-0.39356564809921579</v>
       </c>
       <c r="BA41" s="5">
-        <f>(AX41/AY41-1)*100</f>
+        <f t="shared" si="29"/>
         <v>-2.0600374218786466</v>
       </c>
       <c r="BE41">
-        <f t="shared" ref="BE41:BI41" si="27">(BE38/BE39-1)*100</f>
+        <f t="shared" ref="BE41:BI41" si="35">(BE38/BE39-1)*100</f>
         <v>6.5443107010613399</v>
       </c>
       <c r="BG41">
-        <f t="shared" si="27"/>
+        <f t="shared" si="35"/>
         <v>116.98974493246661</v>
       </c>
       <c r="BI41">
-        <f t="shared" si="27"/>
+        <f t="shared" si="35"/>
         <v>55.143386931114314</v>
       </c>
     </row>
@@ -4284,11 +4368,11 @@
         <v>18.904530166296727</v>
       </c>
       <c r="AZ42" s="5">
-        <f>AX42-AY42</f>
+        <f t="shared" si="28"/>
         <v>10.424598217110233</v>
       </c>
       <c r="BA42" s="5">
-        <f>(AX42/AY42-1)*100</f>
+        <f t="shared" si="29"/>
         <v>55.143386931114314</v>
       </c>
     </row>
@@ -4739,7 +4823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D6:AS41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="AK10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AS23" sqref="AS23:AS25"/>
     </sheetView>
   </sheetViews>
@@ -5090,7 +5174,7 @@
         <v>2.4304879451266799</v>
       </c>
       <c r="AJ10" s="2">
-        <f t="shared" ref="AJ10:AL17" si="0">AVERAGE(D10:AG10)</f>
+        <f t="shared" ref="AJ10:AJ17" si="0">AVERAGE(D10:AG10)</f>
         <v>1.6690253864999696</v>
       </c>
       <c r="AK10" s="2">
@@ -5857,7 +5941,7 @@
         <v>2.7973368331242199</v>
       </c>
       <c r="AJ20" s="2">
-        <f t="shared" ref="AJ20:AL35" si="2">AVERAGE(D20:AG20)</f>
+        <f t="shared" ref="AJ20:AJ35" si="2">AVERAGE(D20:AG20)</f>
         <v>3.4727194131047758</v>
       </c>
       <c r="AK20" s="2">
@@ -7219,7 +7303,7 @@
         <v>4.3021631951043702</v>
       </c>
       <c r="AJ38" s="2">
-        <f t="shared" ref="AJ38:AL41" si="4">AVERAGE(D38:AG38)</f>
+        <f t="shared" ref="AJ38:AJ41" si="4">AVERAGE(D38:AG38)</f>
         <v>6.1724764986002869</v>
       </c>
       <c r="AK38" s="2">

</xml_diff>